<commit_message>
update mysql test classes
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -18942,8 +18942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1556" workbookViewId="0">
-      <selection activeCell="H1586" sqref="H1586"/>
+    <sheetView tabSelected="1" topLeftCell="A1301" workbookViewId="0">
+      <selection activeCell="B1308" sqref="B1308:B1387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -53488,7 +53488,7 @@
         <v>4738</v>
       </c>
       <c r="B1280" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1280" s="1" t="s">
         <v>2186</v>
@@ -53517,7 +53517,7 @@
         <v>3968</v>
       </c>
       <c r="B1281" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1281" s="1" t="s">
         <v>2186</v>
@@ -53546,7 +53546,7 @@
         <v>3969</v>
       </c>
       <c r="B1282" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1282" s="1" t="s">
         <v>2186</v>
@@ -53575,7 +53575,7 @@
         <v>3970</v>
       </c>
       <c r="B1283" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1283" s="1" t="s">
         <v>2186</v>
@@ -53604,7 +53604,7 @@
         <v>3971</v>
       </c>
       <c r="B1284" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1284" s="1" t="s">
         <v>2186</v>
@@ -53633,7 +53633,7 @@
         <v>3972</v>
       </c>
       <c r="B1285" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1285" s="1" t="s">
         <v>2186</v>
@@ -53662,7 +53662,7 @@
         <v>3973</v>
       </c>
       <c r="B1286" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1286" s="1" t="s">
         <v>2186</v>
@@ -53691,7 +53691,7 @@
         <v>3974</v>
       </c>
       <c r="B1287" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1287" s="1" t="s">
         <v>2186</v>
@@ -53720,7 +53720,7 @@
         <v>3975</v>
       </c>
       <c r="B1288" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1288" s="1" t="s">
         <v>2186</v>
@@ -53749,7 +53749,7 @@
         <v>3976</v>
       </c>
       <c r="B1289" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1289" s="1" t="s">
         <v>2186</v>
@@ -54300,7 +54300,7 @@
         <v>3993</v>
       </c>
       <c r="B1308" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1308" s="1" t="s">
         <v>2208</v>
@@ -54332,7 +54332,7 @@
         <v>3994</v>
       </c>
       <c r="B1309" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1309" s="1" t="s">
         <v>2211</v>
@@ -54364,7 +54364,7 @@
         <v>3995</v>
       </c>
       <c r="B1310" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1310" s="1" t="s">
         <v>2212</v>
@@ -54396,7 +54396,7 @@
         <v>3996</v>
       </c>
       <c r="B1311" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1311" s="1" t="s">
         <v>2213</v>
@@ -54428,7 +54428,7 @@
         <v>3997</v>
       </c>
       <c r="B1312" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1312" s="1" t="s">
         <v>2214</v>
@@ -54460,7 +54460,7 @@
         <v>3998</v>
       </c>
       <c r="B1313" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1313" s="1" t="s">
         <v>2215</v>
@@ -54492,7 +54492,7 @@
         <v>3999</v>
       </c>
       <c r="B1314" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1314" s="1" t="s">
         <v>2216</v>
@@ -54524,7 +54524,7 @@
         <v>4000</v>
       </c>
       <c r="B1315" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1315" s="1" t="s">
         <v>2217</v>
@@ -54556,7 +54556,7 @@
         <v>4001</v>
       </c>
       <c r="B1316" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1316" s="1" t="s">
         <v>2218</v>
@@ -54588,7 +54588,7 @@
         <v>4002</v>
       </c>
       <c r="B1317" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1317" s="1" t="s">
         <v>2220</v>
@@ -54620,7 +54620,7 @@
         <v>4003</v>
       </c>
       <c r="B1318" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1318" s="1" t="s">
         <v>2221</v>
@@ -54652,7 +54652,7 @@
         <v>4750</v>
       </c>
       <c r="B1319" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1319" s="1" t="s">
         <v>2223</v>
@@ -54684,7 +54684,7 @@
         <v>4004</v>
       </c>
       <c r="B1320" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1320" s="1" t="s">
         <v>2224</v>
@@ -54716,7 +54716,7 @@
         <v>4005</v>
       </c>
       <c r="B1321" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1321" s="1" t="s">
         <v>2225</v>
@@ -54748,7 +54748,7 @@
         <v>4006</v>
       </c>
       <c r="B1322" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1322" s="1" t="s">
         <v>2238</v>
@@ -54780,7 +54780,7 @@
         <v>4752</v>
       </c>
       <c r="B1323" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1323" s="1" t="s">
         <v>2239</v>
@@ -54812,7 +54812,7 @@
         <v>4007</v>
       </c>
       <c r="B1324" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1324" s="1" t="s">
         <v>2240</v>
@@ -54844,7 +54844,7 @@
         <v>4008</v>
       </c>
       <c r="B1325" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1325" s="1" t="s">
         <v>2241</v>
@@ -54876,7 +54876,7 @@
         <v>4009</v>
       </c>
       <c r="B1326" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1326" s="1" t="s">
         <v>2248</v>
@@ -54908,7 +54908,7 @@
         <v>4010</v>
       </c>
       <c r="B1327" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1327" s="1" t="s">
         <v>2242</v>
@@ -54940,7 +54940,7 @@
         <v>4011</v>
       </c>
       <c r="B1328" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1328" s="1" t="s">
         <v>2249</v>
@@ -54972,7 +54972,7 @@
         <v>4012</v>
       </c>
       <c r="B1329" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1329" s="1" t="s">
         <v>2250</v>
@@ -55004,7 +55004,7 @@
         <v>4013</v>
       </c>
       <c r="B1330" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1330" s="1" t="s">
         <v>2252</v>
@@ -55036,7 +55036,7 @@
         <v>4014</v>
       </c>
       <c r="B1331" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1331" s="1" t="s">
         <v>2252</v>
@@ -55068,7 +55068,7 @@
         <v>4015</v>
       </c>
       <c r="B1332" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1332" s="1" t="s">
         <v>2254</v>
@@ -55100,7 +55100,7 @@
         <v>4016</v>
       </c>
       <c r="B1333" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1333" s="1" t="s">
         <v>2256</v>
@@ -55132,7 +55132,7 @@
         <v>4017</v>
       </c>
       <c r="B1334" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1334" s="1" t="s">
         <v>2257</v>
@@ -55164,7 +55164,7 @@
         <v>4748</v>
       </c>
       <c r="B1335" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1335" s="1" t="s">
         <v>2261</v>
@@ -55196,7 +55196,7 @@
         <v>4744</v>
       </c>
       <c r="B1336" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1336" s="1" t="s">
         <v>2267</v>
@@ -55228,7 +55228,7 @@
         <v>4018</v>
       </c>
       <c r="B1337" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1337" s="1" t="s">
         <v>2268</v>
@@ -55260,7 +55260,7 @@
         <v>4019</v>
       </c>
       <c r="B1338" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1338" s="1" t="s">
         <v>2269</v>
@@ -55292,7 +55292,7 @@
         <v>4020</v>
       </c>
       <c r="B1339" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1339" s="1" t="s">
         <v>2272</v>
@@ -55324,7 +55324,7 @@
         <v>4021</v>
       </c>
       <c r="B1340" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1340" s="1" t="s">
         <v>2273</v>
@@ -55356,7 +55356,7 @@
         <v>4022</v>
       </c>
       <c r="B1341" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1341" s="1" t="s">
         <v>2274</v>
@@ -55388,7 +55388,7 @@
         <v>4023</v>
       </c>
       <c r="B1342" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1342" s="1" t="s">
         <v>2275</v>
@@ -55417,7 +55417,7 @@
         <v>4024</v>
       </c>
       <c r="B1343" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1343" s="1" t="s">
         <v>2277</v>
@@ -55449,7 +55449,7 @@
         <v>4025</v>
       </c>
       <c r="B1344" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1344" s="1" t="s">
         <v>2278</v>
@@ -55481,7 +55481,7 @@
         <v>4746</v>
       </c>
       <c r="B1345" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1345" s="1" t="s">
         <v>2280</v>
@@ -55513,7 +55513,7 @@
         <v>4026</v>
       </c>
       <c r="B1346" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1346" s="1" t="s">
         <v>2281</v>
@@ -55545,7 +55545,7 @@
         <v>4027</v>
       </c>
       <c r="B1347" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1347" s="1" t="s">
         <v>2282</v>
@@ -55577,7 +55577,7 @@
         <v>4028</v>
       </c>
       <c r="B1348" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1348" s="1" t="s">
         <v>2283</v>
@@ -55609,7 +55609,7 @@
         <v>4029</v>
       </c>
       <c r="B1349" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1349" s="1" t="s">
         <v>2284</v>
@@ -55641,7 +55641,7 @@
         <v>4030</v>
       </c>
       <c r="B1350" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1350" s="1" t="s">
         <v>2285</v>
@@ -55673,7 +55673,7 @@
         <v>4031</v>
       </c>
       <c r="B1351" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1351" s="1" t="s">
         <v>2297</v>
@@ -55705,7 +55705,7 @@
         <v>4032</v>
       </c>
       <c r="B1352" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1352" s="1" t="s">
         <v>2300</v>
@@ -55737,7 +55737,7 @@
         <v>4033</v>
       </c>
       <c r="B1353" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1353" s="1" t="s">
         <v>2301</v>
@@ -55769,7 +55769,7 @@
         <v>4034</v>
       </c>
       <c r="B1354" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1354" s="1" t="s">
         <v>2302</v>
@@ -55801,7 +55801,7 @@
         <v>4035</v>
       </c>
       <c r="B1355" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1355" s="1" t="s">
         <v>2304</v>
@@ -55833,7 +55833,7 @@
         <v>4036</v>
       </c>
       <c r="B1356" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1356" s="1" t="s">
         <v>2305</v>
@@ -55865,7 +55865,7 @@
         <v>4037</v>
       </c>
       <c r="B1357" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1357" s="1" t="s">
         <v>2305</v>
@@ -55897,7 +55897,7 @@
         <v>4038</v>
       </c>
       <c r="B1358" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1358" s="1" t="s">
         <v>2306</v>
@@ -55929,7 +55929,7 @@
         <v>4039</v>
       </c>
       <c r="B1359" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1359" s="1" t="s">
         <v>2307</v>
@@ -55961,7 +55961,7 @@
         <v>4040</v>
       </c>
       <c r="B1360" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1360" s="1" t="s">
         <v>2308</v>
@@ -55993,7 +55993,7 @@
         <v>4041</v>
       </c>
       <c r="B1361" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1361" s="1" t="s">
         <v>2309</v>
@@ -56025,7 +56025,7 @@
         <v>4042</v>
       </c>
       <c r="B1362" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1362" s="1" t="s">
         <v>2310</v>
@@ -56057,7 +56057,7 @@
         <v>4043</v>
       </c>
       <c r="B1363" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1363" s="1" t="s">
         <v>2311</v>
@@ -56089,7 +56089,7 @@
         <v>4044</v>
       </c>
       <c r="B1364" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1364" s="1" t="s">
         <v>2312</v>
@@ -56121,7 +56121,7 @@
         <v>4045</v>
       </c>
       <c r="B1365" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1365" s="1" t="s">
         <v>2313</v>
@@ -56153,7 +56153,7 @@
         <v>4046</v>
       </c>
       <c r="B1366" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1366" s="1" t="s">
         <v>2355</v>
@@ -56185,7 +56185,7 @@
         <v>4047</v>
       </c>
       <c r="B1367" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1367" s="1" t="s">
         <v>2340</v>
@@ -56217,7 +56217,7 @@
         <v>4048</v>
       </c>
       <c r="B1368" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1368" s="1" t="s">
         <v>2341</v>
@@ -56249,7 +56249,7 @@
         <v>4049</v>
       </c>
       <c r="B1369" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1369" s="1" t="s">
         <v>2346</v>
@@ -56281,7 +56281,7 @@
         <v>4050</v>
       </c>
       <c r="B1370" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1370" s="1" t="s">
         <v>2348</v>
@@ -56313,7 +56313,7 @@
         <v>4051</v>
       </c>
       <c r="B1371" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1371" s="1" t="s">
         <v>2349</v>
@@ -56345,7 +56345,7 @@
         <v>4052</v>
       </c>
       <c r="B1372" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1372" s="1" t="s">
         <v>2351</v>
@@ -56377,7 +56377,7 @@
         <v>4053</v>
       </c>
       <c r="B1373" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1373" s="1" t="s">
         <v>2351</v>
@@ -56409,7 +56409,7 @@
         <v>4054</v>
       </c>
       <c r="B1374" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1374" s="1" t="s">
         <v>2353</v>
@@ -56441,7 +56441,7 @@
         <v>4055</v>
       </c>
       <c r="B1375" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1375" s="1" t="s">
         <v>2377</v>
@@ -56473,7 +56473,7 @@
         <v>4056</v>
       </c>
       <c r="B1376" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1376" s="1" t="s">
         <v>2378</v>
@@ -56505,7 +56505,7 @@
         <v>4057</v>
       </c>
       <c r="B1377" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1377" s="1" t="s">
         <v>2379</v>
@@ -56537,7 +56537,7 @@
         <v>4058</v>
       </c>
       <c r="B1378" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1378" s="1" t="s">
         <v>2380</v>
@@ -56569,7 +56569,7 @@
         <v>4059</v>
       </c>
       <c r="B1379" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1379" s="1" t="s">
         <v>2381</v>
@@ -56601,7 +56601,7 @@
         <v>4060</v>
       </c>
       <c r="B1380" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1380" s="1" t="s">
         <v>2382</v>
@@ -56633,7 +56633,7 @@
         <v>4061</v>
       </c>
       <c r="B1381" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1381" s="1" t="s">
         <v>2383</v>
@@ -56665,7 +56665,7 @@
         <v>4062</v>
       </c>
       <c r="B1382" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1382" s="1" t="s">
         <v>2384</v>
@@ -56697,7 +56697,7 @@
         <v>4063</v>
       </c>
       <c r="B1383" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1383" s="1" t="s">
         <v>2369</v>
@@ -56726,7 +56726,7 @@
         <v>4753</v>
       </c>
       <c r="B1384" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1384" s="1" t="s">
         <v>2369</v>
@@ -56755,7 +56755,7 @@
         <v>4064</v>
       </c>
       <c r="B1385" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1385" s="1" t="s">
         <v>2369</v>
@@ -56784,7 +56784,7 @@
         <v>4065</v>
       </c>
       <c r="B1386" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1386" s="1" t="s">
         <v>2369</v>
@@ -56813,7 +56813,7 @@
         <v>4066</v>
       </c>
       <c r="B1387" s="4" t="s">
-        <v>34</v>
+        <v>5146</v>
       </c>
       <c r="C1387" s="1" t="s">
         <v>2369</v>

</xml_diff>

<commit_message>
add table function cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14243" uniqueCount="5377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14296" uniqueCount="5410">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -18984,6 +18984,128 @@
   </si>
   <si>
     <t>abc~!@#$%^&amp;*()_+=-|][}{;:/.,?&gt;&lt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-查询全表数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1644.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1645</t>
+  </si>
+  <si>
+    <t>dqlc1_1646</t>
+  </si>
+  <si>
+    <t>TableFunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1644</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1644</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,phone from scan($schema7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1645.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1646.csv</t>
+  </si>
+  <si>
+    <t>dqlc1_1647</t>
+  </si>
+  <si>
+    <t>schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-查询指定多个字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema7) where id &gt;5 and id &lt; 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1648</t>
+  </si>
+  <si>
+    <t>scan表函数-表为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-范围条件过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-like过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount from scan($schema1) where address like '%beijing%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1647.csv</t>
+  </si>
+  <si>
+    <t>dqlc1_1649</t>
+  </si>
+  <si>
+    <t>scan多分区表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1648.csv</t>
+  </si>
+  <si>
+    <t>schema10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1649.csv</t>
+  </si>
+  <si>
+    <t>select id,name,age,amount from scan($schema10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -19372,10 +19494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1644"/>
+  <dimension ref="A1:K1650"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1591" workbookViewId="0">
-      <selection activeCell="C1610" sqref="C1610"/>
+    <sheetView tabSelected="1" topLeftCell="A1627" workbookViewId="0">
+      <selection activeCell="J1650" sqref="J1650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -65415,6 +65537,177 @@
         <v>5367</v>
       </c>
       <c r="K1644" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1645" s="1" t="s">
+        <v>5385</v>
+      </c>
+      <c r="B1645" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1645" s="1" t="s">
+        <v>5380</v>
+      </c>
+      <c r="D1645" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1645" s="1" t="s">
+        <v>5377</v>
+      </c>
+      <c r="G1645" s="1" t="s">
+        <v>5378</v>
+      </c>
+      <c r="I1645" s="1" t="s">
+        <v>5379</v>
+      </c>
+      <c r="J1645" s="1" t="s">
+        <v>5381</v>
+      </c>
+      <c r="K1645" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1646" s="1" t="s">
+        <v>5382</v>
+      </c>
+      <c r="B1646" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1646" s="1" t="s">
+        <v>5392</v>
+      </c>
+      <c r="D1646" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1646" s="1" t="s">
+        <v>5377</v>
+      </c>
+      <c r="H1646" s="1" t="s">
+        <v>5386</v>
+      </c>
+      <c r="I1646" s="1" t="s">
+        <v>5387</v>
+      </c>
+      <c r="J1646" s="1" t="s">
+        <v>5388</v>
+      </c>
+      <c r="K1646" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1647" s="1" t="s">
+        <v>5383</v>
+      </c>
+      <c r="B1647" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1647" s="1" t="s">
+        <v>5397</v>
+      </c>
+      <c r="D1647" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1647" s="1" t="s">
+        <v>5377</v>
+      </c>
+      <c r="H1647" s="1" t="s">
+        <v>5386</v>
+      </c>
+      <c r="I1647" s="1" t="s">
+        <v>5393</v>
+      </c>
+      <c r="J1647" s="1" t="s">
+        <v>5389</v>
+      </c>
+      <c r="K1647" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1648" s="1" t="s">
+        <v>5390</v>
+      </c>
+      <c r="B1648" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1648" s="1" t="s">
+        <v>5398</v>
+      </c>
+      <c r="D1648" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1648" s="1" t="s">
+        <v>5391</v>
+      </c>
+      <c r="G1648" s="1" t="s">
+        <v>5396</v>
+      </c>
+      <c r="I1648" s="1" t="s">
+        <v>5399</v>
+      </c>
+      <c r="J1648" s="1" t="s">
+        <v>5400</v>
+      </c>
+      <c r="K1648" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1649" s="1" t="s">
+        <v>5394</v>
+      </c>
+      <c r="B1649" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1649" s="1" t="s">
+        <v>5395</v>
+      </c>
+      <c r="D1649" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1649" s="1" t="s">
+        <v>5403</v>
+      </c>
+      <c r="I1649" s="1" t="s">
+        <v>5404</v>
+      </c>
+      <c r="J1649" s="1" t="s">
+        <v>5405</v>
+      </c>
+      <c r="K1649" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1650" s="1" t="s">
+        <v>5401</v>
+      </c>
+      <c r="B1650" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1650" s="1" t="s">
+        <v>5402</v>
+      </c>
+      <c r="D1650" s="1" t="s">
+        <v>5384</v>
+      </c>
+      <c r="F1650" s="1" t="s">
+        <v>5406</v>
+      </c>
+      <c r="G1650" s="1" t="s">
+        <v>5407</v>
+      </c>
+      <c r="I1650" s="1" t="s">
+        <v>5409</v>
+      </c>
+      <c r="J1650" s="1" t="s">
+        <v>5408</v>
+      </c>
+      <c r="K1650" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more query case about order by added
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14296" uniqueCount="5410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14556" uniqueCount="5521">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -18967,145 +18967,543 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>select * from $schema27 where name like 'test[~@\*=\]/ "\?]%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema27 where address like '__ [!#\%&amp;-\.]%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select 'abc'||'~!@#$%^&amp;*()_+=-|][}{;:/.,?&gt;&lt;'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abc~!@#$%^&amp;*()_+=-|][}{;:/.,?&gt;&lt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-查询全表数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1644.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1645</t>
+  </si>
+  <si>
+    <t>dqlc1_1646</t>
+  </si>
+  <si>
+    <t>TableFunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1644</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1644</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,phone from scan($schema7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1645.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1646.csv</t>
+  </si>
+  <si>
+    <t>dqlc1_1647</t>
+  </si>
+  <si>
+    <t>schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-查询指定多个字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema7) where id &gt;5 and id &lt; 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1648</t>
+  </si>
+  <si>
+    <t>scan表函数-表为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-范围条件过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scan表函数-like过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount from scan($schema1) where address like '%beijing%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1647.csv</t>
+  </si>
+  <si>
+    <t>scan多分区表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from scan($schema1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1648.csv</t>
+  </si>
+  <si>
+    <t>schema10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1649.csv</t>
+  </si>
+  <si>
+    <t>select id,name,age,amount from scan($schema10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1651</t>
+  </si>
+  <si>
+    <t>dqlc1_1652</t>
+  </si>
+  <si>
+    <t>dqlc1_1653</t>
+  </si>
+  <si>
+    <t>dqlc1_1655</t>
+  </si>
+  <si>
+    <t>dqlc1_1656</t>
+  </si>
+  <si>
+    <t>dqlc1_1657</t>
+  </si>
+  <si>
+    <t>dqlc1_1658</t>
+  </si>
+  <si>
+    <t>dqlc1_1659</t>
+  </si>
+  <si>
+    <t>dqlc1_1660</t>
+  </si>
+  <si>
+    <t>dqlc1_1662</t>
+  </si>
+  <si>
+    <t>单分区单主键，查询单个主键字段，通过非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区单主键，查询单个非主键字段，通过非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区单主键，查询单个主键字段，通过非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区单主键，查询单个非主键字段，通过主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区单主键，查询单个非主键字段，通过非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区单主键，查询单个非主键字段，通过主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1663</t>
+  </si>
+  <si>
+    <t>dqlc1_1664</t>
+  </si>
+  <si>
+    <t>dqlc1_1665</t>
+  </si>
+  <si>
+    <t>dqlc1_1666</t>
+  </si>
+  <si>
+    <t>dqlc1_1668</t>
+  </si>
+  <si>
+    <t>dqlc1_1669</t>
+  </si>
+  <si>
+    <t>dqlc1_1670</t>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个非主键字段，通过单个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个非主键字段，通过多个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个非主键字段，通过多个非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个主键字段，通过单个非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询多个主键字段，通过多个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询单个非主键字段，通过单个非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询单个非主键字段，通过单个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询多个非主键字段，通过多个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema6 order by age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1650.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1650</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema6 order by name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1651.csv</t>
+  </si>
+  <si>
+    <t>select age from $schema6 order by age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1671</t>
+  </si>
+  <si>
+    <t>单分区单主键，查询单个主键字段，通过主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema6 order by name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询单个主键字段，通过多个非主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个主键字段，通过多个主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1652.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1653.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1654.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1655.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1656.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1657.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1658.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1659.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1660.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1661.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1662.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1663.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1664.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1665.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1666.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1667.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1668.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1669.csv</t>
+  </si>
+  <si>
+    <t>schema9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1654</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区单主键，查询单个主键字段，通过主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区单主键，查询主键和非主键字段，排序字段和查询字段相同</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1672</t>
+  </si>
+  <si>
+    <t>dqlc1_1673</t>
+  </si>
+  <si>
+    <t>多分区单主键，查询主键和非主键字段，排序字段和查询字段不相同</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1674</t>
+  </si>
+  <si>
+    <t>多分区单主键，查询单个主键字段，通过主键和非主键排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id from $schema9 order by id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id from $schema9 order by id,name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name from $schema9 order by id,name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name from $schema9 order by id,age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id from $schema9 order by name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema9 order by id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1670.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1671.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1672.csv</t>
+  </si>
+  <si>
+    <t>select amount from $schema9 order by name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1661</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区多主键，查询单个主键字段，通过同主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time from $schema4 order by update_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询单个主键字段，通过单个不同主键值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema4 order by birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select address from $schema4 order by amount desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select address from $schema4 order by age,create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id from $schema4 order by id,name,update_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time from $schema4 order by id,name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1649</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1667</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select DIMENSION from $schema32 where metric_id&gt;=5 order by metric_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select metric_id from $schema32 order by gmt,phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select phone from $schema32 order by DIMENSION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select byte_array from $schema32 order by gmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select dimension,metric_id from $schema32 order by metric_id,dimension</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt,phone from $schema32 order by dimension,metric_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询主键和非主键，通过其他主键和非主键排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区多主键，查询主键和非主键，通过多个非主键排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1675</t>
+  </si>
+  <si>
+    <t>多分区多主键，查询主键和非主键，通过非主键绝对值排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select dimension,phone from $schema32 order by metric_id,gmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select metric_id,gmt,phone from $schema32 order by abs(gmt),phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select metric_id,gmt,phone from $schema32 order by gmt,phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1673.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1674.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1675.csv</t>
+  </si>
+  <si>
     <t>select * from $schema27 where name like binary 'test__'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $schema27 where name like 'test[~@\*=\]/ "\?]%'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $schema27 where address like '__ [!#\%&amp;-\.]%'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select 'abc'||'~!@#$%^&amp;*()_+=-|][}{;:/.,?&gt;&lt;'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>abc~!@#$%^&amp;*()_+=-|][}{;:/.,?&gt;&lt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>schema7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qc1_value11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from scan($schema7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scan表函数-查询全表数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1644.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dqlc1_1645</t>
-  </si>
-  <si>
-    <t>dqlc1_1646</t>
-  </si>
-  <si>
-    <t>TableFunc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dqlc1_1644</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dqlc1_1644</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,name,phone from scan($schema7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1645.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1646.csv</t>
-  </si>
-  <si>
-    <t>dqlc1_1647</t>
-  </si>
-  <si>
-    <t>schema1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scan表函数-查询指定多个字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from scan($schema7) where id &gt;5 and id &lt; 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dqlc1_1648</t>
-  </si>
-  <si>
-    <t>scan表函数-表为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qc1_value01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scan表函数-范围条件过滤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scan表函数-like过滤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select amount from scan($schema1) where address like '%beijing%'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1647.csv</t>
-  </si>
-  <si>
-    <t>dqlc1_1649</t>
-  </si>
-  <si>
-    <t>scan多分区表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>schema1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from scan($schema1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1648.csv</t>
-  </si>
-  <si>
-    <t>schema10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qc1_value13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/TableFunction/queryc1_1649.csv</t>
-  </si>
-  <si>
-    <t>select id,name,age,amount from scan($schema10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -19494,23 +19892,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1650"/>
+  <dimension ref="A1:K1676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1627" workbookViewId="0">
-      <selection activeCell="J1650" sqref="J1650"/>
+    <sheetView tabSelected="1" topLeftCell="A1636" workbookViewId="0">
+      <selection activeCell="G1651" sqref="G1651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="53.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="72.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.125" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
@@ -20051,10 +20449,10 @@
         <v>136</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>5374</v>
+      </c>
+      <c r="J21" t="s">
         <v>5375</v>
-      </c>
-      <c r="J21" t="s">
-        <v>5376</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>9</v>
@@ -65473,7 +65871,7 @@
         <v>5293</v>
       </c>
       <c r="I1642" s="1" t="s">
-        <v>5372</v>
+        <v>5520</v>
       </c>
       <c r="J1642" s="1" t="s">
         <v>5365</v>
@@ -65502,7 +65900,7 @@
         <v>5293</v>
       </c>
       <c r="I1643" s="1" t="s">
-        <v>5373</v>
+        <v>5372</v>
       </c>
       <c r="J1643" s="1" t="s">
         <v>5366</v>
@@ -65531,7 +65929,7 @@
         <v>5293</v>
       </c>
       <c r="I1644" s="1" t="s">
-        <v>5374</v>
+        <v>5373</v>
       </c>
       <c r="J1644" s="1" t="s">
         <v>5367</v>
@@ -65542,28 +65940,28 @@
     </row>
     <row r="1645" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1645" s="1" t="s">
-        <v>5385</v>
+        <v>5384</v>
       </c>
       <c r="B1645" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1645" s="1" t="s">
+        <v>5379</v>
+      </c>
+      <c r="D1645" s="1" t="s">
+        <v>5383</v>
+      </c>
+      <c r="F1645" s="1" t="s">
+        <v>5376</v>
+      </c>
+      <c r="G1645" s="1" t="s">
+        <v>5377</v>
+      </c>
+      <c r="I1645" s="1" t="s">
+        <v>5378</v>
+      </c>
+      <c r="J1645" s="1" t="s">
         <v>5380</v>
-      </c>
-      <c r="D1645" s="1" t="s">
-        <v>5384</v>
-      </c>
-      <c r="F1645" s="1" t="s">
-        <v>5377</v>
-      </c>
-      <c r="G1645" s="1" t="s">
-        <v>5378</v>
-      </c>
-      <c r="I1645" s="1" t="s">
-        <v>5379</v>
-      </c>
-      <c r="J1645" s="1" t="s">
-        <v>5381</v>
       </c>
       <c r="K1645" s="1" t="s">
         <v>44</v>
@@ -65571,28 +65969,28 @@
     </row>
     <row r="1646" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1646" s="1" t="s">
-        <v>5382</v>
+        <v>5381</v>
       </c>
       <c r="B1646" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1646" s="1" t="s">
-        <v>5392</v>
+        <v>5391</v>
       </c>
       <c r="D1646" s="1" t="s">
-        <v>5384</v>
+        <v>5383</v>
       </c>
       <c r="F1646" s="1" t="s">
-        <v>5377</v>
+        <v>5376</v>
       </c>
       <c r="H1646" s="1" t="s">
+        <v>5385</v>
+      </c>
+      <c r="I1646" s="1" t="s">
         <v>5386</v>
       </c>
-      <c r="I1646" s="1" t="s">
+      <c r="J1646" s="1" t="s">
         <v>5387</v>
-      </c>
-      <c r="J1646" s="1" t="s">
-        <v>5388</v>
       </c>
       <c r="K1646" s="1" t="s">
         <v>44</v>
@@ -65600,28 +65998,28 @@
     </row>
     <row r="1647" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1647" s="1" t="s">
+        <v>5382</v>
+      </c>
+      <c r="B1647" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1647" s="1" t="s">
+        <v>5396</v>
+      </c>
+      <c r="D1647" s="1" t="s">
         <v>5383</v>
       </c>
-      <c r="B1647" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1647" s="1" t="s">
-        <v>5397</v>
-      </c>
-      <c r="D1647" s="1" t="s">
-        <v>5384</v>
-      </c>
       <c r="F1647" s="1" t="s">
-        <v>5377</v>
+        <v>5376</v>
       </c>
       <c r="H1647" s="1" t="s">
-        <v>5386</v>
+        <v>5385</v>
       </c>
       <c r="I1647" s="1" t="s">
-        <v>5393</v>
+        <v>5392</v>
       </c>
       <c r="J1647" s="1" t="s">
-        <v>5389</v>
+        <v>5388</v>
       </c>
       <c r="K1647" s="1" t="s">
         <v>44</v>
@@ -65629,28 +66027,28 @@
     </row>
     <row r="1648" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1648" s="1" t="s">
+        <v>5389</v>
+      </c>
+      <c r="B1648" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1648" s="1" t="s">
+        <v>5397</v>
+      </c>
+      <c r="D1648" s="1" t="s">
+        <v>5383</v>
+      </c>
+      <c r="F1648" s="1" t="s">
         <v>5390</v>
       </c>
-      <c r="B1648" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1648" s="1" t="s">
+      <c r="G1648" s="1" t="s">
+        <v>5395</v>
+      </c>
+      <c r="I1648" s="1" t="s">
         <v>5398</v>
       </c>
-      <c r="D1648" s="1" t="s">
-        <v>5384</v>
-      </c>
-      <c r="F1648" s="1" t="s">
-        <v>5391</v>
-      </c>
-      <c r="G1648" s="1" t="s">
-        <v>5396</v>
-      </c>
-      <c r="I1648" s="1" t="s">
+      <c r="J1648" s="1" t="s">
         <v>5399</v>
-      </c>
-      <c r="J1648" s="1" t="s">
-        <v>5400</v>
       </c>
       <c r="K1648" s="1" t="s">
         <v>44</v>
@@ -65658,25 +66056,25 @@
     </row>
     <row r="1649" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1649" s="1" t="s">
+        <v>5393</v>
+      </c>
+      <c r="B1649" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1649" s="1" t="s">
         <v>5394</v>
       </c>
-      <c r="B1649" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1649" s="1" t="s">
-        <v>5395</v>
-      </c>
       <c r="D1649" s="1" t="s">
-        <v>5384</v>
+        <v>5383</v>
       </c>
       <c r="F1649" s="1" t="s">
+        <v>5401</v>
+      </c>
+      <c r="I1649" s="1" t="s">
+        <v>5402</v>
+      </c>
+      <c r="J1649" s="1" t="s">
         <v>5403</v>
-      </c>
-      <c r="I1649" s="1" t="s">
-        <v>5404</v>
-      </c>
-      <c r="J1649" s="1" t="s">
-        <v>5405</v>
       </c>
       <c r="K1649" s="1" t="s">
         <v>44</v>
@@ -65684,31 +66082,863 @@
     </row>
     <row r="1650" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1650" s="1" t="s">
-        <v>5401</v>
+        <v>5500</v>
       </c>
       <c r="B1650" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1650" s="1" t="s">
-        <v>5402</v>
+        <v>5400</v>
       </c>
       <c r="D1650" s="1" t="s">
-        <v>5384</v>
+        <v>5383</v>
       </c>
       <c r="F1650" s="1" t="s">
+        <v>5404</v>
+      </c>
+      <c r="G1650" s="1" t="s">
+        <v>2173</v>
+      </c>
+      <c r="I1650" s="1" t="s">
         <v>5406</v>
       </c>
-      <c r="G1650" s="1" t="s">
-        <v>5407</v>
-      </c>
-      <c r="I1650" s="1" t="s">
-        <v>5409</v>
-      </c>
       <c r="J1650" s="1" t="s">
-        <v>5408</v>
+        <v>5405</v>
       </c>
       <c r="K1650" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1651" s="1" t="s">
+        <v>5442</v>
+      </c>
+      <c r="B1651" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1651" s="1" t="s">
+        <v>5417</v>
+      </c>
+      <c r="D1651" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1651" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1651" s="1" t="s">
+        <v>5438</v>
+      </c>
+      <c r="G1651" s="1" t="s">
+        <v>5439</v>
+      </c>
+      <c r="I1651" s="1" t="s">
+        <v>5440</v>
+      </c>
+      <c r="J1651" s="1" t="s">
+        <v>5441</v>
+      </c>
+      <c r="K1651" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1652" s="1" t="s">
+        <v>5407</v>
+      </c>
+      <c r="B1652" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1652" s="1" t="s">
+        <v>5422</v>
+      </c>
+      <c r="D1652" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1652" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1652" s="1" t="s">
+        <v>5438</v>
+      </c>
+      <c r="H1652" s="1" t="s">
+        <v>5442</v>
+      </c>
+      <c r="I1652" s="1" t="s">
+        <v>5443</v>
+      </c>
+      <c r="J1652" s="1" t="s">
+        <v>5444</v>
+      </c>
+      <c r="K1652" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1653" s="1" t="s">
+        <v>5408</v>
+      </c>
+      <c r="B1653" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1653" s="1" t="s">
+        <v>5418</v>
+      </c>
+      <c r="D1653" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1653" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1653" s="1" t="s">
+        <v>5438</v>
+      </c>
+      <c r="H1653" s="1" t="s">
+        <v>5442</v>
+      </c>
+      <c r="I1653" s="1" t="s">
+        <v>5445</v>
+      </c>
+      <c r="J1653" s="1" t="s">
+        <v>5451</v>
+      </c>
+      <c r="K1653" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1654" s="1" t="s">
+        <v>5409</v>
+      </c>
+      <c r="B1654" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1654" s="1" t="s">
+        <v>5447</v>
+      </c>
+      <c r="D1654" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1654" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1654" s="1" t="s">
+        <v>5438</v>
+      </c>
+      <c r="H1654" s="1" t="s">
+        <v>5442</v>
+      </c>
+      <c r="I1654" s="1" t="s">
+        <v>5448</v>
+      </c>
+      <c r="J1654" s="1" t="s">
+        <v>5452</v>
+      </c>
+      <c r="K1654" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1655" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="B1655" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1655" s="1" t="s">
+        <v>5472</v>
+      </c>
+      <c r="D1655" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1655" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1655" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="G1655" s="1" t="s">
+        <v>5470</v>
+      </c>
+      <c r="I1655" s="1" t="s">
+        <v>5479</v>
+      </c>
+      <c r="J1655" s="1" t="s">
+        <v>5453</v>
+      </c>
+      <c r="K1655" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1656" s="1" t="s">
+        <v>5410</v>
+      </c>
+      <c r="B1656" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1656" s="1" t="s">
+        <v>5478</v>
+      </c>
+      <c r="D1656" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1656" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1656" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1656" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1656" s="1" t="s">
+        <v>5480</v>
+      </c>
+      <c r="J1656" s="1" t="s">
+        <v>5454</v>
+      </c>
+      <c r="K1656" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1657" s="1" t="s">
+        <v>5411</v>
+      </c>
+      <c r="B1657" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1657" s="1" t="s">
+        <v>5473</v>
+      </c>
+      <c r="D1657" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1657" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1657" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1657" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1657" s="1" t="s">
+        <v>5481</v>
+      </c>
+      <c r="J1657" s="1" t="s">
+        <v>5455</v>
+      </c>
+      <c r="K1657" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1658" s="1" t="s">
+        <v>5412</v>
+      </c>
+      <c r="B1658" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1658" s="1" t="s">
+        <v>5476</v>
+      </c>
+      <c r="D1658" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1658" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1658" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1658" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1658" s="1" t="s">
+        <v>5482</v>
+      </c>
+      <c r="J1658" s="1" t="s">
+        <v>5456</v>
+      </c>
+      <c r="K1658" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1659" s="1" t="s">
+        <v>5413</v>
+      </c>
+      <c r="B1659" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1659" s="1" t="s">
+        <v>5419</v>
+      </c>
+      <c r="D1659" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1659" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1659" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1659" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1659" s="1" t="s">
+        <v>5483</v>
+      </c>
+      <c r="J1659" s="1" t="s">
+        <v>5457</v>
+      </c>
+      <c r="K1659" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1660" s="1" t="s">
+        <v>5414</v>
+      </c>
+      <c r="B1660" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1660" s="1" t="s">
+        <v>5420</v>
+      </c>
+      <c r="D1660" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1660" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1660" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1660" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1660" s="1" t="s">
+        <v>5484</v>
+      </c>
+      <c r="J1660" s="1" t="s">
+        <v>5458</v>
+      </c>
+      <c r="K1660" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1661" s="1" t="s">
+        <v>5415</v>
+      </c>
+      <c r="B1661" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1661" s="1" t="s">
+        <v>5421</v>
+      </c>
+      <c r="D1661" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1661" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1661" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="H1661" s="1" t="s">
+        <v>5471</v>
+      </c>
+      <c r="I1661" s="1" t="s">
+        <v>5488</v>
+      </c>
+      <c r="J1661" s="1" t="s">
+        <v>5459</v>
+      </c>
+      <c r="K1661" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1662" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="B1662" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1662" s="1" t="s">
+        <v>5492</v>
+      </c>
+      <c r="D1662" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1662" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1662" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="G1662" s="1" t="s">
+        <v>5490</v>
+      </c>
+      <c r="I1662" s="1" t="s">
+        <v>5493</v>
+      </c>
+      <c r="J1662" s="1" t="s">
+        <v>5460</v>
+      </c>
+      <c r="K1662" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1663" s="1" t="s">
+        <v>5416</v>
+      </c>
+      <c r="B1663" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1663" s="1" t="s">
+        <v>5433</v>
+      </c>
+      <c r="D1663" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1663" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1663" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="H1663" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="I1663" s="1" t="s">
+        <v>5495</v>
+      </c>
+      <c r="J1663" s="1" t="s">
+        <v>5461</v>
+      </c>
+      <c r="K1663" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1664" s="1" t="s">
+        <v>5423</v>
+      </c>
+      <c r="B1664" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1664" s="1" t="s">
+        <v>5430</v>
+      </c>
+      <c r="D1664" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1664" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1664" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="H1664" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="I1664" s="1" t="s">
+        <v>5496</v>
+      </c>
+      <c r="J1664" s="1" t="s">
+        <v>5462</v>
+      </c>
+      <c r="K1664" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1665" s="1" t="s">
+        <v>5424</v>
+      </c>
+      <c r="B1665" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1665" s="1" t="s">
+        <v>5432</v>
+      </c>
+      <c r="D1665" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1665" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1665" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="H1665" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="I1665" s="1" t="s">
+        <v>5497</v>
+      </c>
+      <c r="J1665" s="1" t="s">
+        <v>5463</v>
+      </c>
+      <c r="K1665" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1666" s="1" t="s">
+        <v>5425</v>
+      </c>
+      <c r="B1666" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1666" s="1" t="s">
+        <v>5450</v>
+      </c>
+      <c r="D1666" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1666" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1666" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="H1666" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="I1666" s="1" t="s">
+        <v>5498</v>
+      </c>
+      <c r="J1666" s="1" t="s">
+        <v>5464</v>
+      </c>
+      <c r="K1666" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1667" s="1" t="s">
+        <v>5426</v>
+      </c>
+      <c r="B1667" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1667" s="1" t="s">
+        <v>5431</v>
+      </c>
+      <c r="D1667" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1667" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1667" s="1" t="s">
+        <v>5489</v>
+      </c>
+      <c r="H1667" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="I1667" s="1" t="s">
+        <v>5499</v>
+      </c>
+      <c r="J1667" s="1" t="s">
+        <v>5465</v>
+      </c>
+      <c r="K1667" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1668" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="B1668" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1668" s="1" t="s">
+        <v>5494</v>
+      </c>
+      <c r="D1668" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1668" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1668" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="G1668" s="1" t="s">
+        <v>5501</v>
+      </c>
+      <c r="I1668" s="1" t="s">
+        <v>5504</v>
+      </c>
+      <c r="J1668" s="1" t="s">
+        <v>5466</v>
+      </c>
+      <c r="K1668" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1669" s="1" t="s">
+        <v>5427</v>
+      </c>
+      <c r="B1669" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1669" s="1" t="s">
+        <v>5449</v>
+      </c>
+      <c r="D1669" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1669" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1669" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1669" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1669" s="1" t="s">
+        <v>5505</v>
+      </c>
+      <c r="J1669" s="1" t="s">
+        <v>5467</v>
+      </c>
+      <c r="K1669" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1670" s="1" t="s">
+        <v>5428</v>
+      </c>
+      <c r="B1670" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1670" s="1" t="s">
+        <v>5436</v>
+      </c>
+      <c r="D1670" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1670" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1670" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1670" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1670" s="1" t="s">
+        <v>5506</v>
+      </c>
+      <c r="J1670" s="1" t="s">
+        <v>5468</v>
+      </c>
+      <c r="K1670" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1671" s="1" t="s">
+        <v>5429</v>
+      </c>
+      <c r="B1671" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1671" s="1" t="s">
+        <v>5435</v>
+      </c>
+      <c r="D1671" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1671" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1671" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1671" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1671" s="1" t="s">
+        <v>5507</v>
+      </c>
+      <c r="J1671" s="1" t="s">
+        <v>5485</v>
+      </c>
+      <c r="K1671" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1672" s="1" t="s">
+        <v>5446</v>
+      </c>
+      <c r="B1672" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1672" s="1" t="s">
+        <v>5434</v>
+      </c>
+      <c r="D1672" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1672" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1672" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1672" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1672" s="1" t="s">
+        <v>5508</v>
+      </c>
+      <c r="J1672" s="1" t="s">
+        <v>5486</v>
+      </c>
+      <c r="K1672" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1673" s="1" t="s">
+        <v>5474</v>
+      </c>
+      <c r="B1673" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1673" s="1" t="s">
+        <v>5437</v>
+      </c>
+      <c r="D1673" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1673" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1673" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1673" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1673" s="1" t="s">
+        <v>5509</v>
+      </c>
+      <c r="J1673" s="1" t="s">
+        <v>5487</v>
+      </c>
+      <c r="K1673" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1674" s="1" t="s">
+        <v>5475</v>
+      </c>
+      <c r="B1674" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1674" s="1" t="s">
+        <v>5511</v>
+      </c>
+      <c r="D1674" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1674" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1674" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1674" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1674" s="1" t="s">
+        <v>5516</v>
+      </c>
+      <c r="J1674" s="1" t="s">
+        <v>5517</v>
+      </c>
+      <c r="K1674" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1675" s="1" t="s">
+        <v>5477</v>
+      </c>
+      <c r="B1675" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1675" s="1" t="s">
+        <v>5510</v>
+      </c>
+      <c r="D1675" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1675" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1675" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1675" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1675" s="1" t="s">
+        <v>5514</v>
+      </c>
+      <c r="J1675" s="1" t="s">
+        <v>5518</v>
+      </c>
+      <c r="K1675" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1676" s="1" t="s">
+        <v>5512</v>
+      </c>
+      <c r="B1676" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1676" s="1" t="s">
+        <v>5513</v>
+      </c>
+      <c r="D1676" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E1676" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="F1676" s="1" t="s">
+        <v>5503</v>
+      </c>
+      <c r="H1676" s="1" t="s">
+        <v>5502</v>
+      </c>
+      <c r="I1676" s="1" t="s">
+        <v>5515</v>
+      </c>
+      <c r="J1676" s="1" t="s">
+        <v>5519</v>
+      </c>
+      <c r="K1676" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expected result about some case of float type updated
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19903,7 +19903,7 @@
   <dimension ref="A1:K1676"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1642" workbookViewId="0">
-      <selection activeCell="F1674" sqref="F1674"/>
+      <selection activeCell="C1648" sqref="C1648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -65951,7 +65951,7 @@
         <v>5384</v>
       </c>
       <c r="B1645" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1645" s="1" t="s">
         <v>5379</v>
@@ -65980,7 +65980,7 @@
         <v>5381</v>
       </c>
       <c r="B1646" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1646" s="1" t="s">
         <v>5391</v>
@@ -66009,7 +66009,7 @@
         <v>5382</v>
       </c>
       <c r="B1647" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1647" s="1" t="s">
         <v>5396</v>
@@ -66038,7 +66038,7 @@
         <v>5389</v>
       </c>
       <c r="B1648" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1648" s="1" t="s">
         <v>5397</v>
@@ -66067,7 +66067,7 @@
         <v>5393</v>
       </c>
       <c r="B1649" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1649" s="1" t="s">
         <v>5394</v>
@@ -66093,7 +66093,7 @@
         <v>5500</v>
       </c>
       <c r="B1650" s="1" t="s">
-        <v>34</v>
+        <v>5133</v>
       </c>
       <c r="C1650" s="1" t="s">
         <v>5400</v>

</xml_diff>

<commit_message>
add different type of primary key equal and range query
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14666" uniqueCount="5572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15224" uniqueCount="5851">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -19688,6 +19688,993 @@
   </si>
   <si>
     <t>select count(*) cn from $mixindex017 where id not between 199 and 600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1688</t>
+  </si>
+  <si>
+    <t>dqlc1_1689</t>
+  </si>
+  <si>
+    <t>dqlc1_1691</t>
+  </si>
+  <si>
+    <t>dqlc1_1692</t>
+  </si>
+  <si>
+    <t>dqlc1_1694</t>
+  </si>
+  <si>
+    <t>dqlc1_1695</t>
+  </si>
+  <si>
+    <t>dqlc1_1697</t>
+  </si>
+  <si>
+    <t>dqlc1_1698</t>
+  </si>
+  <si>
+    <t>dqlc1_1700</t>
+  </si>
+  <si>
+    <t>dqlc1_1701</t>
+  </si>
+  <si>
+    <t>dqlc1_1702</t>
+  </si>
+  <si>
+    <t>dqlc1_1704</t>
+  </si>
+  <si>
+    <t>dqlc1_1706</t>
+  </si>
+  <si>
+    <t>dqlc1_1707</t>
+  </si>
+  <si>
+    <t>dqlc1_1709</t>
+  </si>
+  <si>
+    <t>dqlc1_1710</t>
+  </si>
+  <si>
+    <t>单分区-bigint型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-bigint型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-bigint型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-float型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-float型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-float型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-double型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-double型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-double型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-date型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-date型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-date型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-time型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-time型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-time型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-timestamp型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-timestamp型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-timestamp型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-boolean型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1712</t>
+  </si>
+  <si>
+    <t>dqlc1_1713</t>
+  </si>
+  <si>
+    <t>dqlc1_1715</t>
+  </si>
+  <si>
+    <t>dqlc1_1716</t>
+  </si>
+  <si>
+    <t>dqlc1_1718</t>
+  </si>
+  <si>
+    <t>dqlc1_1719</t>
+  </si>
+  <si>
+    <t>dqlc1_1720</t>
+  </si>
+  <si>
+    <t>dqlc1_1721</t>
+  </si>
+  <si>
+    <t>dqlc1_1722</t>
+  </si>
+  <si>
+    <t>dqlc1_1723</t>
+  </si>
+  <si>
+    <t>dqlc1_1724</t>
+  </si>
+  <si>
+    <t>dqlc1_1725</t>
+  </si>
+  <si>
+    <t>dqlc1_1726</t>
+  </si>
+  <si>
+    <t>dqlc1_1727</t>
+  </si>
+  <si>
+    <t>dqlc1_1728</t>
+  </si>
+  <si>
+    <t>dqlc1_1729</t>
+  </si>
+  <si>
+    <t>dqlc1_1730</t>
+  </si>
+  <si>
+    <t>schema34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1687.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1688.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1689.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1690.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1691.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1692.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1693.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1694.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1695.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1696.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1697.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1698.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1699.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1700.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1701.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1702.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1703.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1704.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1705.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1706.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1707.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1708.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1709.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1710.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1711.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1712.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1713.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1714.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1715.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1716.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1717.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1718.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1719.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1720.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1721.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1722.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1723.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1724.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1725.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1726.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1727.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1728.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1729.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1730.csv</t>
+  </si>
+  <si>
+    <t>select uuid from $schema34 where uuid='jboYh0AF-U4kq-ElLx-KePC-E9XK14LtRyWS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1687</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select uuid from $schema34 where uuid&lt;'Zero'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select uuid from $schema34 where uuid&gt;'Zero'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt from $schema35 where gmt=58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1690</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt from $schema35 where gmt&gt;58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt from $schema35 where gmt&lt;58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1693</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price from $schema36 where price=605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price from $schema36 where price&gt;605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price from $schema36 where price&lt;605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema37</t>
+  </si>
+  <si>
+    <t>dqlc1_1696</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1731</t>
+  </si>
+  <si>
+    <t>dqlc1_1732</t>
+  </si>
+  <si>
+    <t>dqlc1_1733</t>
+  </si>
+  <si>
+    <t>dqlc1_1734</t>
+  </si>
+  <si>
+    <t>dqlc1_1735</t>
+  </si>
+  <si>
+    <t>dqlc1_1736</t>
+  </si>
+  <si>
+    <t>单分区-int型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-int型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-int型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1731.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1732.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1733.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1734.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1735.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1736.csv</t>
+  </si>
+  <si>
+    <t>select amount from $schema37 where amount=122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount from $schema37 where amount&gt;122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount from $schema37 where amount&lt;122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema38</t>
+  </si>
+  <si>
+    <t>dqlc1_1699</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday from $schema38 where birthday='2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday from $schema38 where birthday&gt;'2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday from $schema38 where birthday&lt;'2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema39</t>
+  </si>
+  <si>
+    <t>dqlc1_1703</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time from $schema39 where create_time='12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time from $schema39 where create_time&gt;'12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time from $schema39 where create_time&lt;'12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema40</t>
+  </si>
+  <si>
+    <t>dqlc1_1705</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema41</t>
+  </si>
+  <si>
+    <t>dqlc1_1708</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema41 where age=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time from $schema40 where update_time='2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time from $schema40 where update_time&gt;'2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time from $schema40 where update_time&lt;'2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema41 where age&gt;50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema41 where age&lt;50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1737</t>
+  </si>
+  <si>
+    <t>dqlc1_1738</t>
+  </si>
+  <si>
+    <t>dqlc1_1739</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1737.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1738.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1739.csv</t>
+  </si>
+  <si>
+    <t>单分区-字符型主键等值查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-字符型主键大于范围查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-字符型主键小于范围查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-字符型主键等值查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-字符型主键大于范围查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-字符型主键小于范围查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1740</t>
+  </si>
+  <si>
+    <t>dqlc1_1741</t>
+  </si>
+  <si>
+    <t>单分区-boolean型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单分区-boolean型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema43</t>
+  </si>
+  <si>
+    <t>dqlc1_1711</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1714</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1714</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select is_delete from $schema42 where is_delete=true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select is_delete from $schema42 where is_delete&gt;true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select is_delete from $schema42 where is_delete&lt;true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1740.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1741.csv</t>
+  </si>
+  <si>
+    <t>select name from $schema43 where name='ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema43 where name&gt;'ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema43 where name&lt;'ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键等值查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键大于范围查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键小于范围查询 - 首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-bigint型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-bigint型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-bigint型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-float型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-float型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-float型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-double型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-double型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-double型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-date型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-date型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-date型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-time型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-time型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-time型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-timestamp型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-timestamp型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1742</t>
+  </si>
+  <si>
+    <t>dqlc1_1743</t>
+  </si>
+  <si>
+    <t>dqlc1_1744</t>
+  </si>
+  <si>
+    <t>dqlc1_1745</t>
+  </si>
+  <si>
+    <t>dqlc1_1746</t>
+  </si>
+  <si>
+    <t>hash分区-timestamp型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-int型主键等值查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-int型主键大于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-int型主键小于范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键等值查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键大于范围查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash分区-字符型主键小于范围查询 - 非首列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1742.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1743.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1744.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1745.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1746.csv</t>
+  </si>
+  <si>
+    <t>schema44</t>
+  </si>
+  <si>
+    <t>schema45</t>
+  </si>
+  <si>
+    <t>schema46</t>
+  </si>
+  <si>
+    <t>schema47</t>
+  </si>
+  <si>
+    <t>schema48</t>
+  </si>
+  <si>
+    <t>schema49</t>
+  </si>
+  <si>
+    <t>schema50</t>
+  </si>
+  <si>
+    <t>schema51</t>
+  </si>
+  <si>
+    <t>schema52</t>
+  </si>
+  <si>
+    <t>schema53</t>
+  </si>
+  <si>
+    <t>dqlc1_1717</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1720</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1723</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1726</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1729</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1732</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1735</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1738</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1741</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过主键字段等值查询非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过主键字段大于查询非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过主键字段小于查询非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select uuid,gmt from $schema44 where uuid='jboYh0AF-U4kq-ElLx-KePC-E9XK14LtRyWS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select uuid,gmt from $schema44 where uuid&gt;'jboYh0AF-U4kq-ElLx-KePC-E9XK14LtRyWS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema44 where uuid&lt;'jboYh0AF-U4kq-ElLx-KePC-E9XK14LtRyWS'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt,name from $schema45 where gmt=58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select gmt,name from $schema45 where gmt&gt;58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema45 where gmt&lt;58150934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price,age from $schema46 where price=605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price,age from $schema46 where price&gt;605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema46 where price&lt;605.77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount,birthday from $schema47 where amount=122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select amount,birthday from $schema47 where amount&gt;122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema47 where amount&lt;122076.4086</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday,address from $schema48 where birthday='2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday,address from $schema48 where birthday&gt;'2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema48 where birthday&lt;'2000-07-27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time,zip_code from $schema49 where create_time='12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select create_time,zip_code from $schema49 where create_time&gt;'12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema49 where create_time&lt;'12:07:47'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time,price from $schema50 where update_time='2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time,price from $schema50 where update_time&gt;'2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema50 where update_time&lt;'2002-09-09 11:05:38'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age,name from $schema51 where age=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age,name from $schema51 where age&gt;50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema51 where age&lt;50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name,amount from $schema52 where name='ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name,amount from $schema52 where name&gt;'ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema52 where name&lt;'ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema52 where name='ME50'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select uuid from $schema52 where name&gt;'ME50' order by uuid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday,amount from $schema52 where name&lt;'ME50' order by name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1747</t>
+  </si>
+  <si>
+    <t>hash分区-boolean型主键count查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(is_delete) ci from $schema53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1747.csv</t>
+  </si>
+  <si>
+    <t>dqlc1_1748</t>
+  </si>
+  <si>
+    <t>通过主键字段like查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1748.csv</t>
+  </si>
+  <si>
+    <t>select name from $schema52 where name like 'c6%'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20076,10 +21063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1687"/>
+  <dimension ref="A1:K1749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1655" workbookViewId="0">
-      <selection activeCell="C1695" sqref="C1695"/>
+    <sheetView tabSelected="1" topLeftCell="A888" workbookViewId="0">
+      <selection activeCell="G1749" sqref="G1749"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -67475,6 +68462,1804 @@
       </c>
       <c r="K1687" s="1" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1688" s="1" t="s">
+        <v>5671</v>
+      </c>
+      <c r="B1688" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1688" s="1" t="s">
+        <v>5733</v>
+      </c>
+      <c r="D1688" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1688" s="1" t="s">
+        <v>5624</v>
+      </c>
+      <c r="G1688" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1688" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="J1688" s="1" t="s">
+        <v>5626</v>
+      </c>
+      <c r="K1688" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1689" s="1" t="s">
+        <v>5572</v>
+      </c>
+      <c r="B1689" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1689" s="1" t="s">
+        <v>5734</v>
+      </c>
+      <c r="D1689" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1689" s="1" t="s">
+        <v>5624</v>
+      </c>
+      <c r="H1689" s="1" t="s">
+        <v>5671</v>
+      </c>
+      <c r="I1689" s="1" t="s">
+        <v>5672</v>
+      </c>
+      <c r="J1689" s="1" t="s">
+        <v>5627</v>
+      </c>
+      <c r="K1689" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1690" s="1" t="s">
+        <v>5573</v>
+      </c>
+      <c r="B1690" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1690" s="1" t="s">
+        <v>5735</v>
+      </c>
+      <c r="D1690" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1690" s="1" t="s">
+        <v>5624</v>
+      </c>
+      <c r="H1690" s="1" t="s">
+        <v>5671</v>
+      </c>
+      <c r="I1690" s="1" t="s">
+        <v>5673</v>
+      </c>
+      <c r="J1690" s="1" t="s">
+        <v>5628</v>
+      </c>
+      <c r="K1690" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1691" s="1" t="s">
+        <v>5676</v>
+      </c>
+      <c r="B1691" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1691" s="1" t="s">
+        <v>5588</v>
+      </c>
+      <c r="D1691" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1691" s="1" t="s">
+        <v>5674</v>
+      </c>
+      <c r="G1691" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1691" s="1" t="s">
+        <v>5675</v>
+      </c>
+      <c r="J1691" s="1" t="s">
+        <v>5629</v>
+      </c>
+      <c r="K1691" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1692" s="1" t="s">
+        <v>5574</v>
+      </c>
+      <c r="B1692" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1692" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D1692" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1692" s="1" t="s">
+        <v>5674</v>
+      </c>
+      <c r="H1692" s="1" t="s">
+        <v>5676</v>
+      </c>
+      <c r="I1692" s="1" t="s">
+        <v>5677</v>
+      </c>
+      <c r="J1692" s="1" t="s">
+        <v>5630</v>
+      </c>
+      <c r="K1692" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1693" s="1" t="s">
+        <v>5575</v>
+      </c>
+      <c r="B1693" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1693" s="1" t="s">
+        <v>5590</v>
+      </c>
+      <c r="D1693" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1693" s="1" t="s">
+        <v>5674</v>
+      </c>
+      <c r="H1693" s="1" t="s">
+        <v>5676</v>
+      </c>
+      <c r="I1693" s="1" t="s">
+        <v>5678</v>
+      </c>
+      <c r="J1693" s="1" t="s">
+        <v>5631</v>
+      </c>
+      <c r="K1693" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1694" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="B1694" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1694" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="D1694" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1694" s="1" t="s">
+        <v>5679</v>
+      </c>
+      <c r="G1694" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1694" s="1" t="s">
+        <v>5681</v>
+      </c>
+      <c r="J1694" s="1" t="s">
+        <v>5632</v>
+      </c>
+      <c r="K1694" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1695" s="1" t="s">
+        <v>5576</v>
+      </c>
+      <c r="B1695" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1695" s="1" t="s">
+        <v>5592</v>
+      </c>
+      <c r="D1695" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1695" s="1" t="s">
+        <v>5679</v>
+      </c>
+      <c r="H1695" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="I1695" s="1" t="s">
+        <v>5682</v>
+      </c>
+      <c r="J1695" s="1" t="s">
+        <v>5633</v>
+      </c>
+      <c r="K1695" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1696" s="1" t="s">
+        <v>5577</v>
+      </c>
+      <c r="B1696" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1696" s="1" t="s">
+        <v>5593</v>
+      </c>
+      <c r="D1696" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1696" s="1" t="s">
+        <v>5679</v>
+      </c>
+      <c r="H1696" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="I1696" s="1" t="s">
+        <v>5683</v>
+      </c>
+      <c r="J1696" s="1" t="s">
+        <v>5634</v>
+      </c>
+      <c r="K1696" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1697" s="1" t="s">
+        <v>5685</v>
+      </c>
+      <c r="B1697" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1697" s="1" t="s">
+        <v>5594</v>
+      </c>
+      <c r="D1697" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1697" s="1" t="s">
+        <v>5684</v>
+      </c>
+      <c r="G1697" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1697" s="1" t="s">
+        <v>5701</v>
+      </c>
+      <c r="J1697" s="1" t="s">
+        <v>5635</v>
+      </c>
+      <c r="K1697" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1698" s="1" t="s">
+        <v>5578</v>
+      </c>
+      <c r="B1698" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1698" s="1" t="s">
+        <v>5595</v>
+      </c>
+      <c r="D1698" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1698" s="1" t="s">
+        <v>5684</v>
+      </c>
+      <c r="H1698" s="1" t="s">
+        <v>5685</v>
+      </c>
+      <c r="I1698" s="1" t="s">
+        <v>5702</v>
+      </c>
+      <c r="J1698" s="1" t="s">
+        <v>5636</v>
+      </c>
+      <c r="K1698" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1699" s="1" t="s">
+        <v>5579</v>
+      </c>
+      <c r="B1699" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1699" s="1" t="s">
+        <v>5596</v>
+      </c>
+      <c r="D1699" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1699" s="1" t="s">
+        <v>5684</v>
+      </c>
+      <c r="H1699" s="1" t="s">
+        <v>5685</v>
+      </c>
+      <c r="I1699" s="1" t="s">
+        <v>5703</v>
+      </c>
+      <c r="J1699" s="1" t="s">
+        <v>5637</v>
+      </c>
+      <c r="K1699" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1700" s="1" t="s">
+        <v>5705</v>
+      </c>
+      <c r="B1700" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1700" s="1" t="s">
+        <v>5597</v>
+      </c>
+      <c r="D1700" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1700" s="1" t="s">
+        <v>5704</v>
+      </c>
+      <c r="G1700" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1700" s="1" t="s">
+        <v>5706</v>
+      </c>
+      <c r="J1700" s="1" t="s">
+        <v>5638</v>
+      </c>
+      <c r="K1700" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1701" s="1" t="s">
+        <v>5580</v>
+      </c>
+      <c r="B1701" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1701" s="1" t="s">
+        <v>5598</v>
+      </c>
+      <c r="D1701" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1701" s="1" t="s">
+        <v>5704</v>
+      </c>
+      <c r="H1701" s="1" t="s">
+        <v>5705</v>
+      </c>
+      <c r="I1701" s="1" t="s">
+        <v>5707</v>
+      </c>
+      <c r="J1701" s="1" t="s">
+        <v>5639</v>
+      </c>
+      <c r="K1701" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1702" s="1" t="s">
+        <v>5581</v>
+      </c>
+      <c r="B1702" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1702" s="1" t="s">
+        <v>5599</v>
+      </c>
+      <c r="D1702" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1702" s="1" t="s">
+        <v>5704</v>
+      </c>
+      <c r="H1702" s="1" t="s">
+        <v>5705</v>
+      </c>
+      <c r="I1702" s="1" t="s">
+        <v>5708</v>
+      </c>
+      <c r="J1702" s="1" t="s">
+        <v>5640</v>
+      </c>
+      <c r="K1702" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1703" s="1" t="s">
+        <v>5582</v>
+      </c>
+      <c r="B1703" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1703" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="D1703" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1703" s="1" t="s">
+        <v>5709</v>
+      </c>
+      <c r="G1703" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1703" s="1" t="s">
+        <v>5711</v>
+      </c>
+      <c r="J1703" s="1" t="s">
+        <v>5641</v>
+      </c>
+      <c r="K1703" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1704" s="1" t="s">
+        <v>5710</v>
+      </c>
+      <c r="B1704" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1704" s="1" t="s">
+        <v>5601</v>
+      </c>
+      <c r="D1704" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1704" s="1" t="s">
+        <v>5709</v>
+      </c>
+      <c r="H1704" s="1" t="s">
+        <v>5710</v>
+      </c>
+      <c r="I1704" s="1" t="s">
+        <v>5712</v>
+      </c>
+      <c r="J1704" s="1" t="s">
+        <v>5642</v>
+      </c>
+      <c r="K1704" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1705" s="1" t="s">
+        <v>5583</v>
+      </c>
+      <c r="B1705" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1705" s="1" t="s">
+        <v>5602</v>
+      </c>
+      <c r="D1705" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1705" s="1" t="s">
+        <v>5709</v>
+      </c>
+      <c r="H1705" s="1" t="s">
+        <v>5710</v>
+      </c>
+      <c r="I1705" s="1" t="s">
+        <v>5713</v>
+      </c>
+      <c r="J1705" s="1" t="s">
+        <v>5643</v>
+      </c>
+      <c r="K1705" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1706" s="1" t="s">
+        <v>5715</v>
+      </c>
+      <c r="B1706" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1706" s="1" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D1706" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1706" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="G1706" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1706" s="1" t="s">
+        <v>5719</v>
+      </c>
+      <c r="J1706" s="1" t="s">
+        <v>5644</v>
+      </c>
+      <c r="K1706" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1707" s="1" t="s">
+        <v>5584</v>
+      </c>
+      <c r="B1707" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1707" s="1" t="s">
+        <v>5604</v>
+      </c>
+      <c r="D1707" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1707" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="H1707" s="1" t="s">
+        <v>5715</v>
+      </c>
+      <c r="I1707" s="1" t="s">
+        <v>5720</v>
+      </c>
+      <c r="J1707" s="1" t="s">
+        <v>5645</v>
+      </c>
+      <c r="K1707" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1708" s="1" t="s">
+        <v>5585</v>
+      </c>
+      <c r="B1708" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1708" s="1" t="s">
+        <v>5605</v>
+      </c>
+      <c r="D1708" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1708" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="H1708" s="1" t="s">
+        <v>5715</v>
+      </c>
+      <c r="I1708" s="1" t="s">
+        <v>5721</v>
+      </c>
+      <c r="J1708" s="1" t="s">
+        <v>5646</v>
+      </c>
+      <c r="K1708" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1709" s="1" t="s">
+        <v>5717</v>
+      </c>
+      <c r="B1709" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1709" s="1" t="s">
+        <v>5692</v>
+      </c>
+      <c r="D1709" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1709" s="1" t="s">
+        <v>5716</v>
+      </c>
+      <c r="G1709" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1709" s="1" t="s">
+        <v>5718</v>
+      </c>
+      <c r="J1709" s="1" t="s">
+        <v>5647</v>
+      </c>
+      <c r="K1709" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1710" s="1" t="s">
+        <v>5586</v>
+      </c>
+      <c r="B1710" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1710" s="1" t="s">
+        <v>5693</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1710" s="1" t="s">
+        <v>5716</v>
+      </c>
+      <c r="H1710" s="1" t="s">
+        <v>5717</v>
+      </c>
+      <c r="I1710" s="1" t="s">
+        <v>5722</v>
+      </c>
+      <c r="J1710" s="1" t="s">
+        <v>5648</v>
+      </c>
+      <c r="K1710" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1711" s="1" t="s">
+        <v>5587</v>
+      </c>
+      <c r="B1711" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1711" s="1" t="s">
+        <v>5694</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1711" s="1" t="s">
+        <v>5716</v>
+      </c>
+      <c r="H1711" s="1" t="s">
+        <v>5717</v>
+      </c>
+      <c r="I1711" s="1" t="s">
+        <v>5723</v>
+      </c>
+      <c r="J1711" s="1" t="s">
+        <v>5649</v>
+      </c>
+      <c r="K1711" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1712" s="1" t="s">
+        <v>5742</v>
+      </c>
+      <c r="B1712" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1712" s="1" t="s">
+        <v>5606</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1712" s="1" t="s">
+        <v>5736</v>
+      </c>
+      <c r="G1712" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1712" s="1" t="s">
+        <v>5745</v>
+      </c>
+      <c r="J1712" s="1" t="s">
+        <v>5650</v>
+      </c>
+      <c r="K1712" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1713" s="1" t="s">
+        <v>5607</v>
+      </c>
+      <c r="B1713" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1713" s="1" t="s">
+        <v>5739</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1713" s="1" t="s">
+        <v>5736</v>
+      </c>
+      <c r="H1713" s="1" t="s">
+        <v>5742</v>
+      </c>
+      <c r="I1713" s="1" t="s">
+        <v>5746</v>
+      </c>
+      <c r="J1713" s="1" t="s">
+        <v>5651</v>
+      </c>
+      <c r="K1713" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1714" s="1" t="s">
+        <v>5608</v>
+      </c>
+      <c r="B1714" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1714" s="1" t="s">
+        <v>5740</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1714" s="1" t="s">
+        <v>5736</v>
+      </c>
+      <c r="H1714" s="1" t="s">
+        <v>5742</v>
+      </c>
+      <c r="I1714" s="1" t="s">
+        <v>5747</v>
+      </c>
+      <c r="J1714" s="1" t="s">
+        <v>5652</v>
+      </c>
+      <c r="K1714" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1715" s="1" t="s">
+        <v>5743</v>
+      </c>
+      <c r="B1715" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1715" s="1" t="s">
+        <v>5730</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1715" s="1" t="s">
+        <v>5741</v>
+      </c>
+      <c r="G1715" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="I1715" s="1" t="s">
+        <v>5750</v>
+      </c>
+      <c r="J1715" s="1" t="s">
+        <v>5653</v>
+      </c>
+      <c r="K1715" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1716" s="1" t="s">
+        <v>5609</v>
+      </c>
+      <c r="B1716" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1716" s="1" t="s">
+        <v>5731</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1716" s="1" t="s">
+        <v>5741</v>
+      </c>
+      <c r="H1716" s="1" t="s">
+        <v>5744</v>
+      </c>
+      <c r="I1716" s="1" t="s">
+        <v>5751</v>
+      </c>
+      <c r="J1716" s="1" t="s">
+        <v>5654</v>
+      </c>
+      <c r="K1716" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1717" s="1" t="s">
+        <v>5610</v>
+      </c>
+      <c r="B1717" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1717" s="1" t="s">
+        <v>5732</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1717" s="1" t="s">
+        <v>5741</v>
+      </c>
+      <c r="H1717" s="1" t="s">
+        <v>5744</v>
+      </c>
+      <c r="I1717" s="1" t="s">
+        <v>5752</v>
+      </c>
+      <c r="J1717" s="1" t="s">
+        <v>5655</v>
+      </c>
+      <c r="K1717" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1718" s="1" t="s">
+        <v>5800</v>
+      </c>
+      <c r="B1718" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1718" s="1" t="s">
+        <v>5753</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1718" s="1" t="s">
+        <v>5790</v>
+      </c>
+      <c r="G1718" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1718" s="1" t="s">
+        <v>5813</v>
+      </c>
+      <c r="J1718" s="1" t="s">
+        <v>5656</v>
+      </c>
+      <c r="K1718" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1719" s="1" t="s">
+        <v>5611</v>
+      </c>
+      <c r="B1719" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1719" s="1" t="s">
+        <v>5754</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1719" s="1" t="s">
+        <v>5790</v>
+      </c>
+      <c r="H1719" s="1" t="s">
+        <v>5800</v>
+      </c>
+      <c r="I1719" s="1" t="s">
+        <v>5814</v>
+      </c>
+      <c r="J1719" s="1" t="s">
+        <v>5657</v>
+      </c>
+      <c r="K1719" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1720" s="1" t="s">
+        <v>5612</v>
+      </c>
+      <c r="B1720" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1720" s="1" t="s">
+        <v>5755</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1720" s="1" t="s">
+        <v>5790</v>
+      </c>
+      <c r="H1720" s="1" t="s">
+        <v>5800</v>
+      </c>
+      <c r="I1720" s="1" t="s">
+        <v>5815</v>
+      </c>
+      <c r="J1720" s="1" t="s">
+        <v>5658</v>
+      </c>
+      <c r="K1720" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1721" s="1" t="s">
+        <v>5613</v>
+      </c>
+      <c r="B1721" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1721" s="1" t="s">
+        <v>5756</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1721" s="1" t="s">
+        <v>5791</v>
+      </c>
+      <c r="G1721" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1721" s="1" t="s">
+        <v>5816</v>
+      </c>
+      <c r="J1721" s="1" t="s">
+        <v>5659</v>
+      </c>
+      <c r="K1721" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1722" s="1" t="s">
+        <v>5614</v>
+      </c>
+      <c r="B1722" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1722" s="1" t="s">
+        <v>5757</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1722" s="1" t="s">
+        <v>5791</v>
+      </c>
+      <c r="H1722" s="1" t="s">
+        <v>5801</v>
+      </c>
+      <c r="I1722" s="1" t="s">
+        <v>5817</v>
+      </c>
+      <c r="J1722" s="1" t="s">
+        <v>5660</v>
+      </c>
+      <c r="K1722" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1723" s="1" t="s">
+        <v>5615</v>
+      </c>
+      <c r="B1723" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1723" s="1" t="s">
+        <v>5758</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1723" s="1" t="s">
+        <v>5791</v>
+      </c>
+      <c r="H1723" s="1" t="s">
+        <v>5801</v>
+      </c>
+      <c r="I1723" s="1" t="s">
+        <v>5818</v>
+      </c>
+      <c r="J1723" s="1" t="s">
+        <v>5661</v>
+      </c>
+      <c r="K1723" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1724" s="1" t="s">
+        <v>5616</v>
+      </c>
+      <c r="B1724" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1724" s="1" t="s">
+        <v>5759</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1724" s="1" t="s">
+        <v>5792</v>
+      </c>
+      <c r="G1724" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1724" s="1" t="s">
+        <v>5819</v>
+      </c>
+      <c r="J1724" s="1" t="s">
+        <v>5662</v>
+      </c>
+      <c r="K1724" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1725" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="B1725" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1725" s="1" t="s">
+        <v>5760</v>
+      </c>
+      <c r="D1725" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1725" s="1" t="s">
+        <v>5792</v>
+      </c>
+      <c r="H1725" s="1" t="s">
+        <v>5802</v>
+      </c>
+      <c r="I1725" s="1" t="s">
+        <v>5820</v>
+      </c>
+      <c r="J1725" s="1" t="s">
+        <v>5663</v>
+      </c>
+      <c r="K1725" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1726" s="1" t="s">
+        <v>5618</v>
+      </c>
+      <c r="B1726" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1726" s="1" t="s">
+        <v>5761</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1726" s="1" t="s">
+        <v>5792</v>
+      </c>
+      <c r="H1726" s="1" t="s">
+        <v>5802</v>
+      </c>
+      <c r="I1726" s="1" t="s">
+        <v>5821</v>
+      </c>
+      <c r="J1726" s="1" t="s">
+        <v>5664</v>
+      </c>
+      <c r="K1726" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1727" s="1" t="s">
+        <v>5619</v>
+      </c>
+      <c r="B1727" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1727" s="1" t="s">
+        <v>5762</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1727" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="G1727" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1727" s="1" t="s">
+        <v>5822</v>
+      </c>
+      <c r="J1727" s="1" t="s">
+        <v>5665</v>
+      </c>
+      <c r="K1727" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1728" s="1" t="s">
+        <v>5620</v>
+      </c>
+      <c r="B1728" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1728" s="1" t="s">
+        <v>5763</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1728" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="H1728" s="1" t="s">
+        <v>5803</v>
+      </c>
+      <c r="I1728" s="1" t="s">
+        <v>5823</v>
+      </c>
+      <c r="J1728" s="1" t="s">
+        <v>5666</v>
+      </c>
+      <c r="K1728" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1729" s="1" t="s">
+        <v>5621</v>
+      </c>
+      <c r="B1729" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1729" s="1" t="s">
+        <v>5764</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1729" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="H1729" s="1" t="s">
+        <v>5803</v>
+      </c>
+      <c r="I1729" s="1" t="s">
+        <v>5824</v>
+      </c>
+      <c r="J1729" s="1" t="s">
+        <v>5667</v>
+      </c>
+      <c r="K1729" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1730" s="1" t="s">
+        <v>5622</v>
+      </c>
+      <c r="B1730" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1730" s="1" t="s">
+        <v>5765</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1730" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="G1730" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1730" s="1" t="s">
+        <v>5825</v>
+      </c>
+      <c r="J1730" s="1" t="s">
+        <v>5668</v>
+      </c>
+      <c r="K1730" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1731" s="1" t="s">
+        <v>5623</v>
+      </c>
+      <c r="B1731" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1731" s="1" t="s">
+        <v>5766</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1731" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="H1731" s="1" t="s">
+        <v>5804</v>
+      </c>
+      <c r="I1731" s="1" t="s">
+        <v>5826</v>
+      </c>
+      <c r="J1731" s="1" t="s">
+        <v>5669</v>
+      </c>
+      <c r="K1731" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1732" s="1" t="s">
+        <v>5686</v>
+      </c>
+      <c r="B1732" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1732" s="1" t="s">
+        <v>5767</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1732" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="H1732" s="1" t="s">
+        <v>5804</v>
+      </c>
+      <c r="I1732" s="1" t="s">
+        <v>5827</v>
+      </c>
+      <c r="J1732" s="1" t="s">
+        <v>5695</v>
+      </c>
+      <c r="K1732" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1733" s="1" t="s">
+        <v>5687</v>
+      </c>
+      <c r="B1733" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1733" s="1" t="s">
+        <v>5768</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1733" s="1" t="s">
+        <v>5795</v>
+      </c>
+      <c r="G1733" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1733" s="1" t="s">
+        <v>5828</v>
+      </c>
+      <c r="J1733" s="1" t="s">
+        <v>5696</v>
+      </c>
+      <c r="K1733" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1734" s="1" t="s">
+        <v>5688</v>
+      </c>
+      <c r="B1734" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1734" s="1" t="s">
+        <v>5769</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1734" s="1" t="s">
+        <v>5795</v>
+      </c>
+      <c r="H1734" s="1" t="s">
+        <v>5805</v>
+      </c>
+      <c r="I1734" s="1" t="s">
+        <v>5829</v>
+      </c>
+      <c r="J1734" s="1" t="s">
+        <v>5697</v>
+      </c>
+      <c r="K1734" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1735" s="1" t="s">
+        <v>5689</v>
+      </c>
+      <c r="B1735" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1735" s="1" t="s">
+        <v>5770</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1735" s="1" t="s">
+        <v>5795</v>
+      </c>
+      <c r="H1735" s="1" t="s">
+        <v>5805</v>
+      </c>
+      <c r="I1735" s="1" t="s">
+        <v>5830</v>
+      </c>
+      <c r="J1735" s="1" t="s">
+        <v>5698</v>
+      </c>
+      <c r="K1735" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1736" s="1" t="s">
+        <v>5690</v>
+      </c>
+      <c r="B1736" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1736" s="1" t="s">
+        <v>5771</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1736" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="G1736" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1736" s="1" t="s">
+        <v>5831</v>
+      </c>
+      <c r="J1736" s="1" t="s">
+        <v>5699</v>
+      </c>
+      <c r="K1736" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1737" s="1" t="s">
+        <v>5691</v>
+      </c>
+      <c r="B1737" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1737" s="1" t="s">
+        <v>5772</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1737" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="H1737" s="1" t="s">
+        <v>5806</v>
+      </c>
+      <c r="I1737" s="1" t="s">
+        <v>5832</v>
+      </c>
+      <c r="J1737" s="1" t="s">
+        <v>5700</v>
+      </c>
+      <c r="K1737" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1738" s="1" t="s">
+        <v>5724</v>
+      </c>
+      <c r="B1738" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1738" s="1" t="s">
+        <v>5778</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1738" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="H1738" s="1" t="s">
+        <v>5806</v>
+      </c>
+      <c r="I1738" s="1" t="s">
+        <v>5833</v>
+      </c>
+      <c r="J1738" s="1" t="s">
+        <v>5727</v>
+      </c>
+      <c r="K1738" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1739" s="1" t="s">
+        <v>5725</v>
+      </c>
+      <c r="B1739" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1739" s="1" t="s">
+        <v>5779</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1739" s="1" t="s">
+        <v>5797</v>
+      </c>
+      <c r="G1739" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1739" s="1" t="s">
+        <v>5834</v>
+      </c>
+      <c r="J1739" s="1" t="s">
+        <v>5728</v>
+      </c>
+      <c r="K1739" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1740" s="1" t="s">
+        <v>5726</v>
+      </c>
+      <c r="B1740" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1740" s="1" t="s">
+        <v>5780</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1740" s="1" t="s">
+        <v>5797</v>
+      </c>
+      <c r="H1740" s="1" t="s">
+        <v>5807</v>
+      </c>
+      <c r="I1740" s="1" t="s">
+        <v>5835</v>
+      </c>
+      <c r="J1740" s="1" t="s">
+        <v>5729</v>
+      </c>
+      <c r="K1740" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1741" s="1" t="s">
+        <v>5737</v>
+      </c>
+      <c r="B1741" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1741" s="1" t="s">
+        <v>5781</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1741" s="1" t="s">
+        <v>5797</v>
+      </c>
+      <c r="H1741" s="1" t="s">
+        <v>5807</v>
+      </c>
+      <c r="I1741" s="1" t="s">
+        <v>5836</v>
+      </c>
+      <c r="J1741" s="1" t="s">
+        <v>5748</v>
+      </c>
+      <c r="K1741" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1742" s="1" t="s">
+        <v>5738</v>
+      </c>
+      <c r="B1742" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1742" s="1" t="s">
+        <v>5782</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1742" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="G1742" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1742" s="1" t="s">
+        <v>5837</v>
+      </c>
+      <c r="J1742" s="1" t="s">
+        <v>5749</v>
+      </c>
+      <c r="K1742" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1743" s="1" t="s">
+        <v>5773</v>
+      </c>
+      <c r="B1743" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1743" s="1" t="s">
+        <v>5783</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1743" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1743" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1743" s="1" t="s">
+        <v>5838</v>
+      </c>
+      <c r="J1743" s="1" t="s">
+        <v>5785</v>
+      </c>
+      <c r="K1743" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1744" s="1" t="s">
+        <v>5774</v>
+      </c>
+      <c r="B1744" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1744" s="1" t="s">
+        <v>5784</v>
+      </c>
+      <c r="D1744" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1744" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1744" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1744" s="1" t="s">
+        <v>5839</v>
+      </c>
+      <c r="J1744" s="1" t="s">
+        <v>5786</v>
+      </c>
+      <c r="K1744" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1745" s="1" t="s">
+        <v>5775</v>
+      </c>
+      <c r="B1745" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1745" s="1" t="s">
+        <v>5809</v>
+      </c>
+      <c r="D1745" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1745" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1745" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1745" s="1" t="s">
+        <v>5840</v>
+      </c>
+      <c r="J1745" s="1" t="s">
+        <v>5787</v>
+      </c>
+      <c r="K1745" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1746" s="1" t="s">
+        <v>5776</v>
+      </c>
+      <c r="B1746" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1746" s="1" t="s">
+        <v>5810</v>
+      </c>
+      <c r="D1746" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1746" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1746" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1746" s="1" t="s">
+        <v>5841</v>
+      </c>
+      <c r="J1746" s="1" t="s">
+        <v>5788</v>
+      </c>
+      <c r="K1746" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1747" s="1" t="s">
+        <v>5777</v>
+      </c>
+      <c r="B1747" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1747" s="1" t="s">
+        <v>5811</v>
+      </c>
+      <c r="D1747" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1747" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1747" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1747" s="1" t="s">
+        <v>5842</v>
+      </c>
+      <c r="J1747" s="1" t="s">
+        <v>5789</v>
+      </c>
+      <c r="K1747" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1748" s="1" t="s">
+        <v>5843</v>
+      </c>
+      <c r="B1748" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1748" s="1" t="s">
+        <v>5844</v>
+      </c>
+      <c r="D1748" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1748" s="1" t="s">
+        <v>5799</v>
+      </c>
+      <c r="G1748" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="I1748" s="1" t="s">
+        <v>5845</v>
+      </c>
+      <c r="J1748" s="1" t="s">
+        <v>5846</v>
+      </c>
+      <c r="K1748" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1749" s="1" t="s">
+        <v>5847</v>
+      </c>
+      <c r="B1749" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1749" s="1" t="s">
+        <v>5848</v>
+      </c>
+      <c r="D1749" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F1749" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="H1749" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I1749" s="1" t="s">
+        <v>5850</v>
+      </c>
+      <c r="J1749" s="1" t="s">
+        <v>5849</v>
+      </c>
+      <c r="K1749" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync dql test case to mysql
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -21175,8 +21175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1724" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A1604" workbookViewId="0">
+      <selection activeCell="G1622" sqref="G1622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
float equal case query state changes
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -20050,10 +20050,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select price from $schema36 where price&gt;605.77</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select price from $schema36 where price&lt;605.77</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -20554,10 +20550,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select price,age from $schema46 where price&gt;605.77</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select * from $schema46 where price&lt;605.77</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -20798,6 +20790,14 @@
   </si>
   <si>
     <t>select $mixindex010_1.id,$mixindex010_1.age from $mixindex010_0 right join $mixindex010_1 on $mixindex010_0.age=$mixindex010_1.age where $mixindex010_1.age=35 and $mixindex010_0.name='p'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price from $schema36 where price&gt;605.771</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price,age from $schema46 where price&gt;605.771</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -21175,8 +21175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1604" workbookViewId="0">
-      <selection activeCell="G1622" sqref="G1622"/>
+    <sheetView tabSelected="1" topLeftCell="E1703" workbookViewId="0">
+      <selection activeCell="I1726" sqref="I1726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -58692,7 +58692,7 @@
         <v>4734</v>
       </c>
       <c r="I1375" s="1" t="s">
-        <v>5876</v>
+        <v>5874</v>
       </c>
       <c r="J1375" s="1" t="s">
         <v>4562</v>
@@ -68582,7 +68582,7 @@
         <v>34</v>
       </c>
       <c r="C1688" s="1" t="s">
-        <v>5732</v>
+        <v>5731</v>
       </c>
       <c r="D1688" s="1" t="s">
         <v>2410</v>
@@ -68611,7 +68611,7 @@
         <v>34</v>
       </c>
       <c r="C1689" s="1" t="s">
-        <v>5733</v>
+        <v>5732</v>
       </c>
       <c r="D1689" s="1" t="s">
         <v>2410</v>
@@ -68640,7 +68640,7 @@
         <v>34</v>
       </c>
       <c r="C1690" s="1" t="s">
-        <v>5734</v>
+        <v>5733</v>
       </c>
       <c r="D1690" s="1" t="s">
         <v>2410</v>
@@ -68797,7 +68797,7 @@
         <v>5679</v>
       </c>
       <c r="I1695" s="1" t="s">
-        <v>5681</v>
+        <v>5882</v>
       </c>
       <c r="J1695" s="1" t="s">
         <v>5632</v>
@@ -68826,7 +68826,7 @@
         <v>5679</v>
       </c>
       <c r="I1696" s="1" t="s">
-        <v>5682</v>
+        <v>5681</v>
       </c>
       <c r="J1696" s="1" t="s">
         <v>5633</v>
@@ -68837,7 +68837,7 @@
     </row>
     <row r="1697" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1697" s="1" t="s">
-        <v>5684</v>
+        <v>5683</v>
       </c>
       <c r="B1697" s="1" t="s">
         <v>34</v>
@@ -68849,13 +68849,13 @@
         <v>2410</v>
       </c>
       <c r="F1697" s="1" t="s">
-        <v>5683</v>
+        <v>5682</v>
       </c>
       <c r="G1697" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1697" s="1" t="s">
-        <v>5700</v>
+        <v>5699</v>
       </c>
       <c r="J1697" s="1" t="s">
         <v>5634</v>
@@ -68878,13 +68878,13 @@
         <v>2410</v>
       </c>
       <c r="F1698" s="1" t="s">
+        <v>5682</v>
+      </c>
+      <c r="H1698" s="1" t="s">
         <v>5683</v>
       </c>
-      <c r="H1698" s="1" t="s">
-        <v>5684</v>
-      </c>
       <c r="I1698" s="1" t="s">
-        <v>5701</v>
+        <v>5700</v>
       </c>
       <c r="J1698" s="1" t="s">
         <v>5635</v>
@@ -68907,13 +68907,13 @@
         <v>2410</v>
       </c>
       <c r="F1699" s="1" t="s">
+        <v>5682</v>
+      </c>
+      <c r="H1699" s="1" t="s">
         <v>5683</v>
       </c>
-      <c r="H1699" s="1" t="s">
-        <v>5684</v>
-      </c>
       <c r="I1699" s="1" t="s">
-        <v>5702</v>
+        <v>5701</v>
       </c>
       <c r="J1699" s="1" t="s">
         <v>5636</v>
@@ -68924,7 +68924,7 @@
     </row>
     <row r="1700" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1700" s="1" t="s">
-        <v>5704</v>
+        <v>5703</v>
       </c>
       <c r="B1700" s="1" t="s">
         <v>34</v>
@@ -68936,13 +68936,13 @@
         <v>2410</v>
       </c>
       <c r="F1700" s="1" t="s">
-        <v>5703</v>
+        <v>5702</v>
       </c>
       <c r="G1700" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1700" s="1" t="s">
-        <v>5705</v>
+        <v>5704</v>
       </c>
       <c r="J1700" s="1" t="s">
         <v>5637</v>
@@ -68965,13 +68965,13 @@
         <v>2410</v>
       </c>
       <c r="F1701" s="1" t="s">
+        <v>5702</v>
+      </c>
+      <c r="H1701" s="1" t="s">
         <v>5703</v>
       </c>
-      <c r="H1701" s="1" t="s">
-        <v>5704</v>
-      </c>
       <c r="I1701" s="1" t="s">
-        <v>5706</v>
+        <v>5705</v>
       </c>
       <c r="J1701" s="1" t="s">
         <v>5638</v>
@@ -68994,13 +68994,13 @@
         <v>2410</v>
       </c>
       <c r="F1702" s="1" t="s">
+        <v>5702</v>
+      </c>
+      <c r="H1702" s="1" t="s">
         <v>5703</v>
       </c>
-      <c r="H1702" s="1" t="s">
-        <v>5704</v>
-      </c>
       <c r="I1702" s="1" t="s">
-        <v>5707</v>
+        <v>5706</v>
       </c>
       <c r="J1702" s="1" t="s">
         <v>5639</v>
@@ -69023,13 +69023,13 @@
         <v>2410</v>
       </c>
       <c r="F1703" s="1" t="s">
-        <v>5708</v>
+        <v>5707</v>
       </c>
       <c r="G1703" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1703" s="1" t="s">
-        <v>5710</v>
+        <v>5709</v>
       </c>
       <c r="J1703" s="1" t="s">
         <v>5640</v>
@@ -69040,7 +69040,7 @@
     </row>
     <row r="1704" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1704" s="1" t="s">
-        <v>5709</v>
+        <v>5708</v>
       </c>
       <c r="B1704" s="1" t="s">
         <v>34</v>
@@ -69052,13 +69052,13 @@
         <v>2410</v>
       </c>
       <c r="F1704" s="1" t="s">
-        <v>5708</v>
+        <v>5707</v>
       </c>
       <c r="H1704" s="1" t="s">
-        <v>5850</v>
+        <v>5848</v>
       </c>
       <c r="I1704" s="1" t="s">
-        <v>5711</v>
+        <v>5710</v>
       </c>
       <c r="J1704" s="1" t="s">
         <v>5641</v>
@@ -69081,13 +69081,13 @@
         <v>2410</v>
       </c>
       <c r="F1705" s="1" t="s">
-        <v>5708</v>
+        <v>5707</v>
       </c>
       <c r="H1705" s="1" t="s">
-        <v>5850</v>
+        <v>5848</v>
       </c>
       <c r="I1705" s="1" t="s">
-        <v>5712</v>
+        <v>5711</v>
       </c>
       <c r="J1705" s="1" t="s">
         <v>5642</v>
@@ -69098,7 +69098,7 @@
     </row>
     <row r="1706" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1706" s="1" t="s">
-        <v>5714</v>
+        <v>5713</v>
       </c>
       <c r="B1706" s="1" t="s">
         <v>34</v>
@@ -69110,13 +69110,13 @@
         <v>2410</v>
       </c>
       <c r="F1706" s="1" t="s">
-        <v>5713</v>
+        <v>5712</v>
       </c>
       <c r="G1706" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1706" s="1" t="s">
-        <v>5718</v>
+        <v>5717</v>
       </c>
       <c r="J1706" s="1" t="s">
         <v>5643</v>
@@ -69139,13 +69139,13 @@
         <v>2410</v>
       </c>
       <c r="F1707" s="1" t="s">
+        <v>5712</v>
+      </c>
+      <c r="H1707" s="1" t="s">
         <v>5713</v>
       </c>
-      <c r="H1707" s="1" t="s">
-        <v>5714</v>
-      </c>
       <c r="I1707" s="1" t="s">
-        <v>5719</v>
+        <v>5718</v>
       </c>
       <c r="J1707" s="1" t="s">
         <v>5644</v>
@@ -69168,13 +69168,13 @@
         <v>2410</v>
       </c>
       <c r="F1708" s="1" t="s">
+        <v>5712</v>
+      </c>
+      <c r="H1708" s="1" t="s">
         <v>5713</v>
       </c>
-      <c r="H1708" s="1" t="s">
-        <v>5714</v>
-      </c>
       <c r="I1708" s="1" t="s">
-        <v>5720</v>
+        <v>5719</v>
       </c>
       <c r="J1708" s="1" t="s">
         <v>5645</v>
@@ -69185,25 +69185,25 @@
     </row>
     <row r="1709" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1709" s="1" t="s">
-        <v>5716</v>
+        <v>5715</v>
       </c>
       <c r="B1709" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1709" s="1" t="s">
-        <v>5691</v>
+        <v>5690</v>
       </c>
       <c r="D1709" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1709" s="1" t="s">
-        <v>5715</v>
+        <v>5714</v>
       </c>
       <c r="G1709" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1709" s="1" t="s">
-        <v>5717</v>
+        <v>5716</v>
       </c>
       <c r="J1709" s="1" t="s">
         <v>5646</v>
@@ -69220,19 +69220,19 @@
         <v>34</v>
       </c>
       <c r="C1710" s="1" t="s">
-        <v>5692</v>
+        <v>5691</v>
       </c>
       <c r="D1710" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1710" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="H1710" s="1" t="s">
         <v>5715</v>
       </c>
-      <c r="H1710" s="1" t="s">
-        <v>5716</v>
-      </c>
       <c r="I1710" s="1" t="s">
-        <v>5721</v>
+        <v>5720</v>
       </c>
       <c r="J1710" s="1" t="s">
         <v>5647</v>
@@ -69249,19 +69249,19 @@
         <v>34</v>
       </c>
       <c r="C1711" s="1" t="s">
-        <v>5693</v>
+        <v>5692</v>
       </c>
       <c r="D1711" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1711" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="H1711" s="1" t="s">
         <v>5715</v>
       </c>
-      <c r="H1711" s="1" t="s">
-        <v>5716</v>
-      </c>
       <c r="I1711" s="1" t="s">
-        <v>5722</v>
+        <v>5721</v>
       </c>
       <c r="J1711" s="1" t="s">
         <v>5648</v>
@@ -69272,7 +69272,7 @@
     </row>
     <row r="1712" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1712" s="1" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="B1712" s="1" t="s">
         <v>34</v>
@@ -69284,13 +69284,13 @@
         <v>2410</v>
       </c>
       <c r="F1712" s="1" t="s">
-        <v>5735</v>
+        <v>5734</v>
       </c>
       <c r="G1712" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1712" s="1" t="s">
-        <v>5744</v>
+        <v>5743</v>
       </c>
       <c r="J1712" s="1" t="s">
         <v>5649</v>
@@ -69307,19 +69307,19 @@
         <v>34</v>
       </c>
       <c r="C1713" s="1" t="s">
-        <v>5738</v>
+        <v>5737</v>
       </c>
       <c r="D1713" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1713" s="1" t="s">
-        <v>5735</v>
+        <v>5734</v>
       </c>
       <c r="H1713" s="1" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="I1713" s="1" t="s">
-        <v>5745</v>
+        <v>5744</v>
       </c>
       <c r="J1713" s="1" t="s">
         <v>5650</v>
@@ -69336,19 +69336,19 @@
         <v>34</v>
       </c>
       <c r="C1714" s="1" t="s">
-        <v>5739</v>
+        <v>5738</v>
       </c>
       <c r="D1714" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1714" s="1" t="s">
-        <v>5735</v>
+        <v>5734</v>
       </c>
       <c r="H1714" s="1" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="I1714" s="1" t="s">
-        <v>5746</v>
+        <v>5745</v>
       </c>
       <c r="J1714" s="1" t="s">
         <v>5651</v>
@@ -69359,25 +69359,25 @@
     </row>
     <row r="1715" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1715" s="1" t="s">
-        <v>5742</v>
+        <v>5741</v>
       </c>
       <c r="B1715" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1715" s="1" t="s">
-        <v>5729</v>
+        <v>5728</v>
       </c>
       <c r="D1715" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1715" s="1" t="s">
-        <v>5740</v>
+        <v>5739</v>
       </c>
       <c r="G1715" s="1" t="s">
         <v>5624</v>
       </c>
       <c r="I1715" s="1" t="s">
-        <v>5749</v>
+        <v>5748</v>
       </c>
       <c r="J1715" s="1" t="s">
         <v>5652</v>
@@ -69394,19 +69394,19 @@
         <v>34</v>
       </c>
       <c r="C1716" s="1" t="s">
-        <v>5730</v>
+        <v>5729</v>
       </c>
       <c r="D1716" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1716" s="1" t="s">
-        <v>5740</v>
+        <v>5739</v>
       </c>
       <c r="H1716" s="1" t="s">
-        <v>5743</v>
+        <v>5742</v>
       </c>
       <c r="I1716" s="1" t="s">
-        <v>5750</v>
+        <v>5749</v>
       </c>
       <c r="J1716" s="1" t="s">
         <v>5653</v>
@@ -69423,19 +69423,19 @@
         <v>34</v>
       </c>
       <c r="C1717" s="1" t="s">
-        <v>5731</v>
+        <v>5730</v>
       </c>
       <c r="D1717" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1717" s="1" t="s">
-        <v>5740</v>
+        <v>5739</v>
       </c>
       <c r="H1717" s="1" t="s">
-        <v>5743</v>
+        <v>5742</v>
       </c>
       <c r="I1717" s="1" t="s">
-        <v>5751</v>
+        <v>5750</v>
       </c>
       <c r="J1717" s="1" t="s">
         <v>5654</v>
@@ -69446,25 +69446,25 @@
     </row>
     <row r="1718" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1718" s="1" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="B1718" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1718" s="1" t="s">
-        <v>5752</v>
+        <v>5751</v>
       </c>
       <c r="D1718" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1718" s="1" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="G1718" s="1" t="s">
+        <v>5810</v>
+      </c>
+      <c r="I1718" s="1" t="s">
         <v>5811</v>
-      </c>
-      <c r="I1718" s="1" t="s">
-        <v>5812</v>
       </c>
       <c r="J1718" s="1" t="s">
         <v>5655</v>
@@ -69481,19 +69481,19 @@
         <v>34</v>
       </c>
       <c r="C1719" s="1" t="s">
-        <v>5753</v>
+        <v>5752</v>
       </c>
       <c r="D1719" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1719" s="1" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="H1719" s="1" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="I1719" s="1" t="s">
-        <v>5813</v>
+        <v>5812</v>
       </c>
       <c r="J1719" s="1" t="s">
         <v>5656</v>
@@ -69510,19 +69510,19 @@
         <v>34</v>
       </c>
       <c r="C1720" s="1" t="s">
-        <v>5754</v>
+        <v>5753</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1720" s="1" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="H1720" s="1" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="I1720" s="1" t="s">
-        <v>5814</v>
+        <v>5813</v>
       </c>
       <c r="J1720" s="1" t="s">
         <v>5657</v>
@@ -69539,19 +69539,19 @@
         <v>34</v>
       </c>
       <c r="C1721" s="1" t="s">
-        <v>5755</v>
+        <v>5754</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1721" s="1" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="G1721" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1721" s="1" t="s">
-        <v>5815</v>
+        <v>5814</v>
       </c>
       <c r="J1721" s="1" t="s">
         <v>5658</v>
@@ -69568,19 +69568,19 @@
         <v>34</v>
       </c>
       <c r="C1722" s="1" t="s">
-        <v>5756</v>
+        <v>5755</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1722" s="1" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="H1722" s="1" t="s">
-        <v>5800</v>
+        <v>5799</v>
       </c>
       <c r="I1722" s="1" t="s">
-        <v>5816</v>
+        <v>5815</v>
       </c>
       <c r="J1722" s="1" t="s">
         <v>5659</v>
@@ -69597,19 +69597,19 @@
         <v>34</v>
       </c>
       <c r="C1723" s="1" t="s">
-        <v>5757</v>
+        <v>5756</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1723" s="1" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="H1723" s="1" t="s">
-        <v>5800</v>
+        <v>5799</v>
       </c>
       <c r="I1723" s="1" t="s">
-        <v>5817</v>
+        <v>5816</v>
       </c>
       <c r="J1723" s="1" t="s">
         <v>5660</v>
@@ -69626,19 +69626,19 @@
         <v>34</v>
       </c>
       <c r="C1724" s="1" t="s">
-        <v>5758</v>
+        <v>5757</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1724" s="1" t="s">
-        <v>5791</v>
+        <v>5790</v>
       </c>
       <c r="G1724" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1724" s="1" t="s">
-        <v>5818</v>
+        <v>5817</v>
       </c>
       <c r="J1724" s="1" t="s">
         <v>5661</v>
@@ -69655,19 +69655,19 @@
         <v>34</v>
       </c>
       <c r="C1725" s="1" t="s">
-        <v>5759</v>
+        <v>5758</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1725" s="1" t="s">
-        <v>5791</v>
+        <v>5790</v>
       </c>
       <c r="H1725" s="1" t="s">
-        <v>5801</v>
+        <v>5800</v>
       </c>
       <c r="I1725" s="1" t="s">
-        <v>5819</v>
+        <v>5883</v>
       </c>
       <c r="J1725" s="1" t="s">
         <v>5662</v>
@@ -69684,19 +69684,19 @@
         <v>34</v>
       </c>
       <c r="C1726" s="1" t="s">
-        <v>5760</v>
+        <v>5759</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1726" s="1" t="s">
-        <v>5791</v>
+        <v>5790</v>
       </c>
       <c r="H1726" s="1" t="s">
-        <v>5801</v>
+        <v>5800</v>
       </c>
       <c r="I1726" s="1" t="s">
-        <v>5820</v>
+        <v>5818</v>
       </c>
       <c r="J1726" s="1" t="s">
         <v>5663</v>
@@ -69713,19 +69713,19 @@
         <v>34</v>
       </c>
       <c r="C1727" s="1" t="s">
-        <v>5761</v>
+        <v>5760</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1727" s="1" t="s">
-        <v>5792</v>
+        <v>5791</v>
       </c>
       <c r="G1727" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1727" s="1" t="s">
-        <v>5821</v>
+        <v>5819</v>
       </c>
       <c r="J1727" s="1" t="s">
         <v>5664</v>
@@ -69742,19 +69742,19 @@
         <v>34</v>
       </c>
       <c r="C1728" s="1" t="s">
-        <v>5762</v>
+        <v>5761</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1728" s="1" t="s">
-        <v>5792</v>
+        <v>5791</v>
       </c>
       <c r="H1728" s="1" t="s">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="I1728" s="1" t="s">
-        <v>5822</v>
+        <v>5820</v>
       </c>
       <c r="J1728" s="1" t="s">
         <v>5665</v>
@@ -69771,19 +69771,19 @@
         <v>34</v>
       </c>
       <c r="C1729" s="1" t="s">
-        <v>5763</v>
+        <v>5762</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1729" s="1" t="s">
-        <v>5792</v>
+        <v>5791</v>
       </c>
       <c r="H1729" s="1" t="s">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="I1729" s="1" t="s">
-        <v>5823</v>
+        <v>5821</v>
       </c>
       <c r="J1729" s="1" t="s">
         <v>5666</v>
@@ -69800,19 +69800,19 @@
         <v>34</v>
       </c>
       <c r="C1730" s="1" t="s">
-        <v>5764</v>
+        <v>5763</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1730" s="1" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="G1730" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1730" s="1" t="s">
-        <v>5824</v>
+        <v>5822</v>
       </c>
       <c r="J1730" s="1" t="s">
         <v>5667</v>
@@ -69829,19 +69829,19 @@
         <v>34</v>
       </c>
       <c r="C1731" s="1" t="s">
-        <v>5765</v>
+        <v>5764</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1731" s="1" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="H1731" s="1" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="I1731" s="1" t="s">
-        <v>5825</v>
+        <v>5823</v>
       </c>
       <c r="J1731" s="1" t="s">
         <v>5668</v>
@@ -69852,28 +69852,28 @@
     </row>
     <row r="1732" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1732" s="1" t="s">
-        <v>5685</v>
+        <v>5684</v>
       </c>
       <c r="B1732" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1732" s="1" t="s">
-        <v>5766</v>
+        <v>5765</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1732" s="1" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="H1732" s="1" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="I1732" s="1" t="s">
-        <v>5826</v>
+        <v>5824</v>
       </c>
       <c r="J1732" s="1" t="s">
-        <v>5694</v>
+        <v>5693</v>
       </c>
       <c r="K1732" s="1" t="s">
         <v>44</v>
@@ -69881,28 +69881,28 @@
     </row>
     <row r="1733" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1733" s="1" t="s">
-        <v>5686</v>
+        <v>5685</v>
       </c>
       <c r="B1733" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1733" s="1" t="s">
-        <v>5767</v>
+        <v>5766</v>
       </c>
       <c r="D1733" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1733" s="1" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="G1733" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1733" s="1" t="s">
-        <v>5827</v>
+        <v>5825</v>
       </c>
       <c r="J1733" s="1" t="s">
-        <v>5695</v>
+        <v>5694</v>
       </c>
       <c r="K1733" s="1" t="s">
         <v>44</v>
@@ -69910,28 +69910,28 @@
     </row>
     <row r="1734" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1734" s="1" t="s">
-        <v>5687</v>
+        <v>5686</v>
       </c>
       <c r="B1734" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1734" s="1" t="s">
-        <v>5768</v>
+        <v>5767</v>
       </c>
       <c r="D1734" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1734" s="1" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="H1734" s="1" t="s">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="I1734" s="1" t="s">
-        <v>5828</v>
+        <v>5826</v>
       </c>
       <c r="J1734" s="1" t="s">
-        <v>5696</v>
+        <v>5695</v>
       </c>
       <c r="K1734" s="1" t="s">
         <v>44</v>
@@ -69939,28 +69939,28 @@
     </row>
     <row r="1735" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1735" s="1" t="s">
-        <v>5688</v>
+        <v>5687</v>
       </c>
       <c r="B1735" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1735" s="1" t="s">
-        <v>5769</v>
+        <v>5768</v>
       </c>
       <c r="D1735" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1735" s="1" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="H1735" s="1" t="s">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="I1735" s="1" t="s">
-        <v>5829</v>
+        <v>5827</v>
       </c>
       <c r="J1735" s="1" t="s">
-        <v>5697</v>
+        <v>5696</v>
       </c>
       <c r="K1735" s="1" t="s">
         <v>44</v>
@@ -69968,28 +69968,28 @@
     </row>
     <row r="1736" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1736" s="1" t="s">
-        <v>5689</v>
+        <v>5688</v>
       </c>
       <c r="B1736" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1736" s="1" t="s">
-        <v>5770</v>
+        <v>5769</v>
       </c>
       <c r="D1736" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1736" s="1" t="s">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="G1736" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1736" s="1" t="s">
-        <v>5830</v>
+        <v>5828</v>
       </c>
       <c r="J1736" s="1" t="s">
-        <v>5698</v>
+        <v>5697</v>
       </c>
       <c r="K1736" s="1" t="s">
         <v>44</v>
@@ -69997,28 +69997,28 @@
     </row>
     <row r="1737" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1737" s="1" t="s">
-        <v>5690</v>
+        <v>5689</v>
       </c>
       <c r="B1737" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1737" s="1" t="s">
-        <v>5771</v>
+        <v>5770</v>
       </c>
       <c r="D1737" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1737" s="1" t="s">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="H1737" s="1" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="I1737" s="1" t="s">
-        <v>5831</v>
+        <v>5829</v>
       </c>
       <c r="J1737" s="1" t="s">
-        <v>5699</v>
+        <v>5698</v>
       </c>
       <c r="K1737" s="1" t="s">
         <v>44</v>
@@ -70026,28 +70026,28 @@
     </row>
     <row r="1738" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1738" s="1" t="s">
-        <v>5723</v>
+        <v>5722</v>
       </c>
       <c r="B1738" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1738" s="1" t="s">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="D1738" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1738" s="1" t="s">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="H1738" s="1" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="I1738" s="1" t="s">
-        <v>5832</v>
+        <v>5830</v>
       </c>
       <c r="J1738" s="1" t="s">
-        <v>5726</v>
+        <v>5725</v>
       </c>
       <c r="K1738" s="1" t="s">
         <v>44</v>
@@ -70055,28 +70055,28 @@
     </row>
     <row r="1739" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1739" s="1" t="s">
-        <v>5724</v>
+        <v>5723</v>
       </c>
       <c r="B1739" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1739" s="1" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="D1739" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1739" s="1" t="s">
-        <v>5796</v>
+        <v>5795</v>
       </c>
       <c r="G1739" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1739" s="1" t="s">
-        <v>5833</v>
+        <v>5831</v>
       </c>
       <c r="J1739" s="1" t="s">
-        <v>5727</v>
+        <v>5726</v>
       </c>
       <c r="K1739" s="1" t="s">
         <v>44</v>
@@ -70084,28 +70084,28 @@
     </row>
     <row r="1740" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1740" s="1" t="s">
-        <v>5725</v>
+        <v>5724</v>
       </c>
       <c r="B1740" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1740" s="1" t="s">
-        <v>5779</v>
+        <v>5778</v>
       </c>
       <c r="D1740" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1740" s="1" t="s">
-        <v>5796</v>
+        <v>5795</v>
       </c>
       <c r="H1740" s="1" t="s">
-        <v>5806</v>
+        <v>5805</v>
       </c>
       <c r="I1740" s="1" t="s">
-        <v>5834</v>
+        <v>5832</v>
       </c>
       <c r="J1740" s="1" t="s">
-        <v>5728</v>
+        <v>5727</v>
       </c>
       <c r="K1740" s="1" t="s">
         <v>44</v>
@@ -70113,28 +70113,28 @@
     </row>
     <row r="1741" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1741" s="1" t="s">
-        <v>5736</v>
+        <v>5735</v>
       </c>
       <c r="B1741" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1741" s="1" t="s">
-        <v>5780</v>
+        <v>5779</v>
       </c>
       <c r="D1741" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1741" s="1" t="s">
-        <v>5796</v>
+        <v>5795</v>
       </c>
       <c r="H1741" s="1" t="s">
-        <v>5806</v>
+        <v>5805</v>
       </c>
       <c r="I1741" s="1" t="s">
-        <v>5835</v>
+        <v>5833</v>
       </c>
       <c r="J1741" s="1" t="s">
-        <v>5747</v>
+        <v>5746</v>
       </c>
       <c r="K1741" s="1" t="s">
         <v>44</v>
@@ -70142,28 +70142,28 @@
     </row>
     <row r="1742" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1742" s="1" t="s">
-        <v>5737</v>
+        <v>5736</v>
       </c>
       <c r="B1742" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1742" s="1" t="s">
-        <v>5781</v>
+        <v>5780</v>
       </c>
       <c r="D1742" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1742" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="G1742" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1742" s="1" t="s">
-        <v>5836</v>
+        <v>5834</v>
       </c>
       <c r="J1742" s="1" t="s">
-        <v>5748</v>
+        <v>5747</v>
       </c>
       <c r="K1742" s="1" t="s">
         <v>44</v>
@@ -70171,28 +70171,28 @@
     </row>
     <row r="1743" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1743" s="1" t="s">
-        <v>5772</v>
+        <v>5771</v>
       </c>
       <c r="B1743" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1743" s="1" t="s">
-        <v>5782</v>
+        <v>5781</v>
       </c>
       <c r="D1743" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1743" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1743" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1743" s="1" t="s">
-        <v>5837</v>
+        <v>5835</v>
       </c>
       <c r="J1743" s="1" t="s">
-        <v>5784</v>
+        <v>5783</v>
       </c>
       <c r="K1743" s="1" t="s">
         <v>44</v>
@@ -70200,28 +70200,28 @@
     </row>
     <row r="1744" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1744" s="1" t="s">
-        <v>5773</v>
+        <v>5772</v>
       </c>
       <c r="B1744" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1744" s="1" t="s">
-        <v>5783</v>
+        <v>5782</v>
       </c>
       <c r="D1744" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1744" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1744" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1744" s="1" t="s">
-        <v>5838</v>
+        <v>5836</v>
       </c>
       <c r="J1744" s="1" t="s">
-        <v>5785</v>
+        <v>5784</v>
       </c>
       <c r="K1744" s="1" t="s">
         <v>44</v>
@@ -70229,28 +70229,28 @@
     </row>
     <row r="1745" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1745" s="1" t="s">
-        <v>5774</v>
+        <v>5773</v>
       </c>
       <c r="B1745" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1745" s="1" t="s">
-        <v>5808</v>
+        <v>5807</v>
       </c>
       <c r="D1745" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1745" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1745" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1745" s="1" t="s">
-        <v>5839</v>
+        <v>5837</v>
       </c>
       <c r="J1745" s="1" t="s">
-        <v>5786</v>
+        <v>5785</v>
       </c>
       <c r="K1745" s="1" t="s">
         <v>44</v>
@@ -70258,28 +70258,28 @@
     </row>
     <row r="1746" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1746" s="1" t="s">
-        <v>5775</v>
+        <v>5774</v>
       </c>
       <c r="B1746" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1746" s="1" t="s">
-        <v>5809</v>
+        <v>5808</v>
       </c>
       <c r="D1746" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1746" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1746" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1746" s="1" t="s">
-        <v>5840</v>
+        <v>5838</v>
       </c>
       <c r="J1746" s="1" t="s">
-        <v>5787</v>
+        <v>5786</v>
       </c>
       <c r="K1746" s="1" t="s">
         <v>155</v>
@@ -70287,28 +70287,28 @@
     </row>
     <row r="1747" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1747" s="1" t="s">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="B1747" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1747" s="1" t="s">
-        <v>5810</v>
+        <v>5809</v>
       </c>
       <c r="D1747" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1747" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1747" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1747" s="1" t="s">
-        <v>5841</v>
+        <v>5839</v>
       </c>
       <c r="J1747" s="1" t="s">
-        <v>5788</v>
+        <v>5787</v>
       </c>
       <c r="K1747" s="1" t="s">
         <v>155</v>
@@ -70316,28 +70316,28 @@
     </row>
     <row r="1748" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1748" s="1" t="s">
-        <v>5842</v>
+        <v>5840</v>
       </c>
       <c r="B1748" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1748" s="1" t="s">
-        <v>5843</v>
+        <v>5841</v>
       </c>
       <c r="D1748" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1748" s="1" t="s">
-        <v>5798</v>
+        <v>5797</v>
       </c>
       <c r="G1748" s="1" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="I1748" s="1" t="s">
-        <v>5844</v>
+        <v>5842</v>
       </c>
       <c r="J1748" s="1" t="s">
-        <v>5845</v>
+        <v>5843</v>
       </c>
       <c r="K1748" s="1" t="s">
         <v>155</v>
@@ -70345,28 +70345,28 @@
     </row>
     <row r="1749" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1749" s="1" t="s">
-        <v>5846</v>
+        <v>5844</v>
       </c>
       <c r="B1749" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1749" s="1" t="s">
-        <v>5847</v>
+        <v>5845</v>
       </c>
       <c r="D1749" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="F1749" s="1" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="H1749" s="1" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="I1749" s="1" t="s">
-        <v>5849</v>
+        <v>5847</v>
       </c>
       <c r="J1749" s="1" t="s">
-        <v>5848</v>
+        <v>5846</v>
       </c>
       <c r="K1749" s="1" t="s">
         <v>44</v>
@@ -70374,31 +70374,31 @@
     </row>
     <row r="1750" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1750" s="1" t="s">
-        <v>5861</v>
+        <v>5859</v>
       </c>
       <c r="B1750" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1750" s="1" t="s">
-        <v>5852</v>
+        <v>5850</v>
       </c>
       <c r="D1750" s="1" t="s">
-        <v>5856</v>
+        <v>5854</v>
       </c>
       <c r="E1750" s="1" t="s">
-        <v>5857</v>
+        <v>5855</v>
       </c>
       <c r="F1750" s="1" t="s">
-        <v>5860</v>
+        <v>5858</v>
       </c>
       <c r="G1750" s="1" t="s">
         <v>2135</v>
       </c>
       <c r="I1750" s="1" t="s">
-        <v>5862</v>
+        <v>5860</v>
       </c>
       <c r="J1750" s="1" t="s">
-        <v>5863</v>
+        <v>5861</v>
       </c>
       <c r="K1750" s="1" t="s">
         <v>44</v>
@@ -70406,31 +70406,31 @@
     </row>
     <row r="1751" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1751" s="1" t="s">
+        <v>5849</v>
+      </c>
+      <c r="B1751" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1751" s="1" t="s">
         <v>5851</v>
       </c>
-      <c r="B1751" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1751" s="1" t="s">
-        <v>5853</v>
-      </c>
       <c r="D1751" s="1" t="s">
+        <v>5854</v>
+      </c>
+      <c r="E1751" s="1" t="s">
         <v>5856</v>
       </c>
-      <c r="E1751" s="1" t="s">
+      <c r="F1751" s="1" t="s">
         <v>5858</v>
       </c>
-      <c r="F1751" s="1" t="s">
-        <v>5860</v>
-      </c>
       <c r="H1751" s="1" t="s">
-        <v>5861</v>
+        <v>5859</v>
       </c>
       <c r="I1751" s="1" t="s">
-        <v>5864</v>
+        <v>5862</v>
       </c>
       <c r="J1751" s="1" t="s">
-        <v>5865</v>
+        <v>5863</v>
       </c>
       <c r="K1751" s="1" t="s">
         <v>44</v>
@@ -70438,31 +70438,31 @@
     </row>
     <row r="1752" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1752" s="1" t="s">
+        <v>5852</v>
+      </c>
+      <c r="B1752" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1752" s="1" t="s">
+        <v>5853</v>
+      </c>
+      <c r="D1752" s="1" t="s">
         <v>5854</v>
       </c>
-      <c r="B1752" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1752" s="1" t="s">
-        <v>5855</v>
-      </c>
-      <c r="D1752" s="1" t="s">
-        <v>5856</v>
-      </c>
       <c r="E1752" s="1" t="s">
+        <v>5857</v>
+      </c>
+      <c r="F1752" s="1" t="s">
+        <v>5858</v>
+      </c>
+      <c r="H1752" s="1" t="s">
         <v>5859</v>
       </c>
-      <c r="F1752" s="1" t="s">
-        <v>5860</v>
-      </c>
-      <c r="H1752" s="1" t="s">
-        <v>5861</v>
-      </c>
       <c r="I1752" s="1" t="s">
-        <v>5867</v>
+        <v>5865</v>
       </c>
       <c r="J1752" s="1" t="s">
-        <v>5866</v>
+        <v>5864</v>
       </c>
       <c r="K1752" s="1" t="s">
         <v>44</v>
@@ -70470,13 +70470,13 @@
     </row>
     <row r="1753" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1753" s="1" t="s">
-        <v>5875</v>
+        <v>5873</v>
       </c>
       <c r="B1753" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1753" s="1" t="s">
-        <v>5870</v>
+        <v>5868</v>
       </c>
       <c r="D1753" s="1" t="s">
         <v>2202</v>
@@ -70485,16 +70485,16 @@
         <v>2204</v>
       </c>
       <c r="F1753" s="1" t="s">
-        <v>5877</v>
+        <v>5875</v>
       </c>
       <c r="G1753" s="1" t="s">
-        <v>5874</v>
+        <v>5872</v>
       </c>
       <c r="I1753" s="1" t="s">
+        <v>5876</v>
+      </c>
+      <c r="J1753" s="1" t="s">
         <v>5878</v>
-      </c>
-      <c r="J1753" s="1" t="s">
-        <v>5880</v>
       </c>
       <c r="K1753" s="1" t="s">
         <v>44</v>
@@ -70502,13 +70502,13 @@
     </row>
     <row r="1754" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1754" s="1" t="s">
-        <v>5868</v>
+        <v>5866</v>
       </c>
       <c r="B1754" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1754" s="1" t="s">
-        <v>5871</v>
+        <v>5869</v>
       </c>
       <c r="D1754" s="1" t="s">
         <v>2202</v>
@@ -70517,16 +70517,16 @@
         <v>2294</v>
       </c>
       <c r="F1754" s="1" t="s">
+        <v>5871</v>
+      </c>
+      <c r="H1754" s="1" t="s">
         <v>5873</v>
       </c>
-      <c r="H1754" s="1" t="s">
-        <v>5875</v>
-      </c>
       <c r="I1754" s="1" t="s">
+        <v>5877</v>
+      </c>
+      <c r="J1754" s="1" t="s">
         <v>5879</v>
-      </c>
-      <c r="J1754" s="1" t="s">
-        <v>5881</v>
       </c>
       <c r="K1754" s="1" t="s">
         <v>44</v>
@@ -70534,13 +70534,13 @@
     </row>
     <row r="1755" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1755" s="1" t="s">
-        <v>5869</v>
+        <v>5867</v>
       </c>
       <c r="B1755" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1755" s="1" t="s">
-        <v>5872</v>
+        <v>5870</v>
       </c>
       <c r="D1755" s="1" t="s">
         <v>2202</v>
@@ -70549,16 +70549,16 @@
         <v>2324</v>
       </c>
       <c r="F1755" s="1" t="s">
-        <v>5877</v>
+        <v>5875</v>
       </c>
       <c r="H1755" s="1" t="s">
-        <v>5875</v>
+        <v>5873</v>
       </c>
       <c r="I1755" s="1" t="s">
-        <v>5883</v>
+        <v>5881</v>
       </c>
       <c r="J1755" s="1" t="s">
-        <v>5882</v>
+        <v>5880</v>
       </c>
       <c r="K1755" s="1" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
add case about insertID
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15284" uniqueCount="5884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15293" uniqueCount="5888">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -20798,6 +20798,21 @@
   </si>
   <si>
     <t>select price,age from $schema46 where price&gt;605.771</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1755</t>
+  </si>
+  <si>
+    <t>从数据表中查询常量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select 1 from $schema52 limit 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/SQLFuncs/queryc1_1755.csv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -21173,10 +21188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1755"/>
+  <dimension ref="A1:K1756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1703" workbookViewId="0">
-      <selection activeCell="I1726" sqref="I1726"/>
+    <sheetView tabSelected="1" topLeftCell="A1706" workbookViewId="0">
+      <selection activeCell="F1728" sqref="F1728"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -70562,6 +70577,35 @@
       </c>
       <c r="K1755" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1756" s="1" t="s">
+        <v>5884</v>
+      </c>
+      <c r="B1756" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1756" s="1" t="s">
+        <v>5885</v>
+      </c>
+      <c r="D1756" s="1" t="s">
+        <v>2410</v>
+      </c>
+      <c r="F1756" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="H1756" s="1" t="s">
+        <v>5806</v>
+      </c>
+      <c r="I1756" s="1" t="s">
+        <v>5886</v>
+      </c>
+      <c r="J1756" s="1" t="s">
+        <v>5887</v>
+      </c>
+      <c r="K1756" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize code and split connection for each test class
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/sql_dql_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15554" uniqueCount="5988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15584" uniqueCount="6006">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -21071,10 +21071,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='$schema56' or `TABLE_SCHEMA` in ('MYSQL', 'INFORMATION_SCHEMA')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select abs(9223372036854775807.345)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -21173,6 +21169,77 @@
   <si>
     <t>Json</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='$schema56'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1791</t>
+  </si>
+  <si>
+    <t>ComplexDataType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array22_value59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/ComplexDataType/array/queryc1_1791.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar array字段在中间，通过array后字段条件查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float array字段在中间，通过array后字段条件查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array23</t>
+  </si>
+  <si>
+    <t>array23_value60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $array22 where name='lala'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/ComplexDataType/array/queryc1_1792.csv</t>
+  </si>
+  <si>
+    <t>select user_data,id from $array23 where id&gt;2 or age&gt;20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1793</t>
+  </si>
+  <si>
+    <t>float array字段在中间，通过array后字段条件仅查询主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1792</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1792</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id from $array23 where id&gt;1 and age&gt;20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup1/expectedresult/ComplexDataType/array/queryc1_1793.csv</t>
   </si>
 </sst>
 </file>
@@ -21553,10 +21620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1791"/>
+  <dimension ref="A1:K1794"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1630" workbookViewId="0">
-      <selection activeCell="F1760" sqref="F1760"/>
+    <sheetView tabSelected="1" topLeftCell="E1766" workbookViewId="0">
+      <selection activeCell="I1802" sqref="I1802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21568,7 +21635,7 @@
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="97.25" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.125" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
@@ -22084,7 +22151,7 @@
         <v>136</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>5963</v>
+        <v>5962</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>150</v>
@@ -46884,7 +46951,7 @@
         <v>1680</v>
       </c>
       <c r="I972" s="1" t="s">
-        <v>5961</v>
+        <v>5960</v>
       </c>
       <c r="J972" s="1" t="s">
         <v>1722</v>
@@ -71660,7 +71727,7 @@
         <v>34</v>
       </c>
       <c r="C1786" s="12" t="s">
-        <v>5962</v>
+        <v>5961</v>
       </c>
       <c r="D1786" s="12" t="s">
         <v>5957</v>
@@ -71672,7 +71739,7 @@
       <c r="G1786" s="12"/>
       <c r="H1786" s="12"/>
       <c r="I1786" s="12" t="s">
-        <v>5960</v>
+        <v>5987</v>
       </c>
       <c r="J1786" s="12" t="s">
         <v>5959</v>
@@ -71683,16 +71750,16 @@
     </row>
     <row r="1787" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1787" s="12" t="s">
-        <v>5964</v>
+        <v>5963</v>
       </c>
       <c r="B1787" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C1787" s="1" t="s">
-        <v>5966</v>
+        <v>5965</v>
       </c>
       <c r="D1787" s="1" t="s">
-        <v>5968</v>
+        <v>5967</v>
       </c>
       <c r="F1787" s="12" t="s">
         <v>2126</v>
@@ -71702,10 +71769,10 @@
         <v>4717</v>
       </c>
       <c r="I1787" s="1" t="s">
-        <v>5969</v>
+        <v>5968</v>
       </c>
       <c r="J1787" s="1" t="s">
-        <v>5971</v>
+        <v>5970</v>
       </c>
       <c r="K1787" s="12" t="s">
         <v>44</v>
@@ -71713,16 +71780,16 @@
     </row>
     <row r="1788" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1788" s="12" t="s">
-        <v>5965</v>
+        <v>5964</v>
       </c>
       <c r="B1788" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C1788" s="12" t="s">
+        <v>5966</v>
+      </c>
+      <c r="D1788" s="12" t="s">
         <v>5967</v>
-      </c>
-      <c r="D1788" s="12" t="s">
-        <v>5968</v>
       </c>
       <c r="F1788" s="12" t="s">
         <v>2126</v>
@@ -71732,10 +71799,10 @@
         <v>4717</v>
       </c>
       <c r="I1788" s="1" t="s">
-        <v>5970</v>
+        <v>5969</v>
       </c>
       <c r="J1788" s="12" t="s">
-        <v>5972</v>
+        <v>5971</v>
       </c>
       <c r="K1788" s="12" t="s">
         <v>44</v>
@@ -71743,16 +71810,16 @@
     </row>
     <row r="1789" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1789" s="12" t="s">
+        <v>5972</v>
+      </c>
+      <c r="B1789" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1789" s="12" t="s">
         <v>5973</v>
       </c>
-      <c r="B1789" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1789" s="12" t="s">
-        <v>5974</v>
-      </c>
       <c r="D1789" s="12" t="s">
-        <v>5968</v>
+        <v>5967</v>
       </c>
       <c r="E1789" s="12"/>
       <c r="F1789" s="12" t="s">
@@ -71763,10 +71830,10 @@
         <v>4717</v>
       </c>
       <c r="I1789" s="1" t="s">
+        <v>5974</v>
+      </c>
+      <c r="J1789" s="12" t="s">
         <v>5975</v>
-      </c>
-      <c r="J1789" s="12" t="s">
-        <v>5976</v>
       </c>
       <c r="K1789" s="12" t="s">
         <v>44</v>
@@ -71774,16 +71841,16 @@
     </row>
     <row r="1790" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1790" s="12" t="s">
+        <v>5976</v>
+      </c>
+      <c r="B1790" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1790" s="1" t="s">
         <v>5977</v>
       </c>
-      <c r="B1790" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1790" s="1" t="s">
-        <v>5978</v>
-      </c>
       <c r="D1790" s="12" t="s">
-        <v>5968</v>
+        <v>5967</v>
       </c>
       <c r="F1790" s="12" t="s">
         <v>2126</v>
@@ -71793,10 +71860,10 @@
         <v>4717</v>
       </c>
       <c r="I1790" s="1" t="s">
+        <v>5978</v>
+      </c>
+      <c r="J1790" s="12" t="s">
         <v>5979</v>
-      </c>
-      <c r="J1790" s="12" t="s">
-        <v>5980</v>
       </c>
       <c r="K1790" s="1" t="s">
         <v>154</v>
@@ -71804,33 +71871,129 @@
     </row>
     <row r="1791" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1791" s="12" t="s">
+        <v>5980</v>
+      </c>
+      <c r="B1791" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1791" s="1" t="s">
         <v>5981</v>
-      </c>
-      <c r="B1791" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1791" s="1" t="s">
-        <v>5982</v>
       </c>
       <c r="D1791" s="12" t="s">
         <v>5957</v>
       </c>
       <c r="E1791" s="1" t="s">
-        <v>5987</v>
+        <v>5986</v>
       </c>
       <c r="F1791" s="1" t="s">
+        <v>5982</v>
+      </c>
+      <c r="G1791" s="1" t="s">
         <v>5983</v>
       </c>
-      <c r="G1791" s="1" t="s">
+      <c r="I1791" s="1" t="s">
         <v>5984</v>
       </c>
-      <c r="I1791" s="1" t="s">
+      <c r="J1791" s="1" t="s">
         <v>5985</v>
       </c>
-      <c r="J1791" s="1" t="s">
-        <v>5986</v>
-      </c>
       <c r="K1791" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1792" s="12" t="s">
+        <v>5988</v>
+      </c>
+      <c r="B1792" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1792" s="1" t="s">
+        <v>5993</v>
+      </c>
+      <c r="D1792" s="1" t="s">
+        <v>5989</v>
+      </c>
+      <c r="E1792" s="1" t="s">
+        <v>4744</v>
+      </c>
+      <c r="F1792" s="1" t="s">
+        <v>5990</v>
+      </c>
+      <c r="G1792" s="1" t="s">
+        <v>5991</v>
+      </c>
+      <c r="I1792" s="1" t="s">
+        <v>5997</v>
+      </c>
+      <c r="J1792" s="1" t="s">
+        <v>5992</v>
+      </c>
+      <c r="K1792" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1793" s="12" t="s">
+        <v>6002</v>
+      </c>
+      <c r="B1793" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1793" s="12" t="s">
+        <v>5994</v>
+      </c>
+      <c r="D1793" s="12" t="s">
+        <v>5989</v>
+      </c>
+      <c r="E1793" s="12" t="s">
+        <v>4744</v>
+      </c>
+      <c r="F1793" s="12" t="s">
+        <v>5995</v>
+      </c>
+      <c r="G1793" s="12" t="s">
+        <v>5996</v>
+      </c>
+      <c r="I1793" s="1" t="s">
+        <v>5999</v>
+      </c>
+      <c r="J1793" s="12" t="s">
+        <v>5998</v>
+      </c>
+      <c r="K1793" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1794" s="12" t="s">
+        <v>6000</v>
+      </c>
+      <c r="B1794" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1794" s="12" t="s">
+        <v>6001</v>
+      </c>
+      <c r="D1794" s="12" t="s">
+        <v>5989</v>
+      </c>
+      <c r="E1794" s="12" t="s">
+        <v>4744</v>
+      </c>
+      <c r="F1794" s="12" t="s">
+        <v>5995</v>
+      </c>
+      <c r="H1794" s="1" t="s">
+        <v>6003</v>
+      </c>
+      <c r="I1794" s="12" t="s">
+        <v>6004</v>
+      </c>
+      <c r="J1794" s="12" t="s">
+        <v>6005</v>
+      </c>
+      <c r="K1794" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>